<commit_message>
fixed USD ON index conventions
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_SynthQuotesFeed.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_SynthQuotesFeed.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="-15" windowWidth="19140" windowHeight="12015"/>
+    <workbookView xWindow="19095" yWindow="-15" windowWidth="19140" windowHeight="12015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="4" r:id="rId1"/>
@@ -217,9 +217,6 @@
     <t>USD</t>
   </si>
   <si>
-    <t>FedFund</t>
-  </si>
-  <si>
     <t>UnitedKingdom::Exchange</t>
   </si>
   <si>
@@ -308,6 +305,9 @@
   </si>
   <si>
     <t>6MD</t>
+  </si>
+  <si>
+    <t>USDFedFunds</t>
   </si>
 </sst>
 </file>
@@ -1429,6 +1429,15 @@
     <xf numFmtId="0" fontId="7" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="20" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1446,15 +1455,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="18" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="20" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="23">
@@ -1541,43 +1541,43 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>73</v>
+            <v>89</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8">
-            <v>0</v>
+            <v>2</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="8">
           <cell r="D8" t="str">
-            <v>USDSTD</v>
+            <v>USD1M#0000</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2">
         <row r="7">
           <cell r="D7" t="str">
-            <v>LiborYC3M</v>
+            <v>3M</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8" t="str">
-            <v>LiborYC3M</v>
+            <v>3M</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
         <row r="7">
           <cell r="D7" t="str">
-            <v>LiborYC3M</v>
+            <v>3M</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8" t="str">
-            <v>LiborYC3M</v>
+            <v>3M</v>
           </cell>
         </row>
       </sheetData>
@@ -2131,8 +2131,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2151,23 +2151,23 @@
     <row r="1" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="139" t="str">
         <f>_xll.qlxlVersion(TRUE,EvaluationDate)</f>
-        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Apr 18 2014 11:20:01</v>
+        <v>QuantLibXL 1.4.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Apr 29 2014 14:47:17</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="232" t="s">
+      <c r="B2" s="235" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="234"/>
-      <c r="H2" s="235" t="s">
-        <v>65</v>
-      </c>
-      <c r="I2" s="236"/>
-      <c r="J2" s="236"/>
-      <c r="K2" s="237"/>
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="237"/>
+      <c r="H2" s="238" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="239"/>
+      <c r="J2" s="239"/>
+      <c r="K2" s="240"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B3" s="142"/>
@@ -2192,7 +2192,7 @@
       <c r="F4" s="143"/>
       <c r="H4" s="155"/>
       <c r="I4" s="158" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="159" t="b">
         <v>1</v>
@@ -2206,14 +2206,14 @@
         <v>16</v>
       </c>
       <c r="D5" s="137" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="143"/>
       <c r="G5" s="139"/>
       <c r="H5" s="155"/>
       <c r="I5" s="158" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="159" t="b">
         <v>0</v>
@@ -2260,7 +2260,7 @@
       <c r="G6" s="139"/>
       <c r="H6" s="155"/>
       <c r="I6" s="158" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J6" s="159" t="b">
         <v>0</v>
@@ -2298,13 +2298,13 @@
         <v>27</v>
       </c>
       <c r="D7" s="138" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
       <c r="E7" s="41"/>
       <c r="F7" s="143"/>
       <c r="H7" s="155"/>
       <c r="I7" s="158" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7" s="161"/>
       <c r="K7" s="160"/>
@@ -2312,16 +2312,16 @@
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B8" s="142"/>
       <c r="C8" s="50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="138" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="41"/>
       <c r="F8" s="143"/>
       <c r="H8" s="155"/>
       <c r="I8" s="158" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J8" s="162" t="b">
         <v>1</v>
@@ -2346,23 +2346,23 @@
       </c>
       <c r="D10" s="57">
         <f>_xll.qlCalendarAdvance(Calendar,EvaluationDate,"2D","f")</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="E10" s="41"/>
       <c r="F10" s="143"/>
       <c r="H10" s="155"/>
       <c r="I10" s="158" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="162" t="s">
         <v>71</v>
-      </c>
-      <c r="J10" s="162" t="s">
-        <v>72</v>
       </c>
       <c r="K10" s="160"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B11" s="142"/>
       <c r="C11" s="50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D11" s="57">
         <f>_xll.qlCalendarAdjust(Calendar,DATE(YEAR(SettlementDate),12,31),"Preceding")</f>
@@ -2372,7 +2372,7 @@
       <c r="F11" s="143"/>
       <c r="H11" s="155"/>
       <c r="I11" s="158" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J11" s="163">
         <v>1E-4</v>
@@ -2382,7 +2382,7 @@
     <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B12" s="142"/>
       <c r="C12" s="50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="57">
         <f>_xll.qlCalendarAdjust(Calendar,DATE(YEAR(SettlementDate)+1,12,31),"Preceding")</f>
@@ -2392,7 +2392,7 @@
       <c r="F12" s="143"/>
       <c r="H12" s="155"/>
       <c r="I12" s="158" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J12" s="164">
         <v>-0.01</v>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="D14" s="51" t="str">
         <f>_xll.qlDiscountingSwapEngine(,OisCurve,,,,,EvaluationDate)</f>
-        <v>obj_00274#0000</v>
+        <v>obj_00345#0001</v>
       </c>
       <c r="E14" s="41"/>
       <c r="F14" s="143"/>
@@ -2583,11 +2583,9 @@
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="58"/>
       <c r="B2" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="152">
-        <v>41752.613599537035</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C2" s="152"/>
       <c r="D2" s="59"/>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
@@ -2619,7 +2617,7 @@
       </c>
       <c r="C3" s="151">
         <f>_xll.qlSettingsEvaluationDate(Trigger)</f>
-        <v>41752</v>
+        <v>41761</v>
       </c>
       <c r="D3" s="59"/>
       <c r="E3" s="60"/>
@@ -2680,7 +2678,7 @@
       </c>
       <c r="C5" s="150">
         <f>[1]!TriggerCounter</f>
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="D5" s="59"/>
       <c r="E5" s="60"/>
@@ -2713,7 +2711,7 @@
       </c>
       <c r="C6" s="231">
         <f>[1]!LastFixingsTrigger</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="59"/>
       <c r="E6" s="60"/>
@@ -8049,16 +8047,16 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="17.83203125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="10" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="26.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="17.83203125" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="10" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="32.33203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="6" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="9.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.33203125" style="1"/>
@@ -8132,7 +8130,7 @@
       </c>
       <c r="B2" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E2,F2,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00286#0000</v>
+        <v>obj_0048c#0000</v>
       </c>
       <c r="C2" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B2,OisEngine)</f>
@@ -8144,23 +8142,23 @@
       </c>
       <c r="E2" s="112">
         <f>SettlementDate</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="F2" s="113">
         <f>_xll.qlCalendarAdvance(Calendar,E2,A3,"mf")</f>
-        <v>41786</v>
+        <v>41799</v>
       </c>
       <c r="G2" s="114">
         <f>_xll.qlQuoteValue($D2,AllTriggers)</f>
-        <v>1.5229999999999998E-3</v>
+        <v>1.505E-3</v>
       </c>
       <c r="H2" s="115">
         <f>_xll.qlOvernightIndexedSwapFairRate(B2,_xll.ohTrigger(C2,InterestRatesTrigger))</f>
-        <v>9.109858327968624E-4</v>
+        <v>9.0000000005797563E-4</v>
       </c>
       <c r="I2" s="116">
         <f>G2-H2</f>
-        <v>6.1201416720313743E-4</v>
+        <v>6.0499999994202442E-4</v>
       </c>
       <c r="J2" s="117" t="b">
         <v>0</v>
@@ -8174,33 +8172,33 @@
       </c>
       <c r="O2" s="120">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" s="120">
         <f>(O2^2-N2^2)/(O2-N2)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="117"/>
       <c r="R2" s="131">
         <f>(O2^3-N2^3)/3/(O2-N2)</f>
-        <v>341.33333333333331</v>
+        <v>363</v>
       </c>
       <c r="S2" s="131">
         <f>(O2+N2)/2</f>
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="T2" s="131">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="238" t="str">
+      <c r="A3" s="232" t="str">
         <f>_xll.qlPeriodEquivalent(A2&amp;"M")</f>
         <v>1M</v>
       </c>
       <c r="B3" s="65" t="str">
         <f>_xll.qlMakeDatedOIS(,E3,F3,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00287#0000</v>
+        <v>obj_00491#0000</v>
       </c>
       <c r="C3" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B3,OisEngine)</f>
@@ -8212,23 +8210,23 @@
       </c>
       <c r="E3" s="105">
         <f>E2</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="F3" s="106">
         <f>F2</f>
-        <v>41786</v>
+        <v>41799</v>
       </c>
       <c r="G3" s="107">
         <f>_xll.qlQuoteValue(D3,AllTriggers)</f>
-        <v>1.5229999999999998E-3</v>
+        <v>1.505E-3</v>
       </c>
       <c r="H3" s="108">
         <f>_xll.qlOvernightIndexedSwapFairRate(B3,_xll.ohTrigger(C3,InterestRatesTrigger))</f>
-        <v>9.109858327968624E-4</v>
+        <v>9.0000000005797563E-4</v>
       </c>
       <c r="I3" s="109">
         <f t="shared" ref="I3:I27" si="1">G3-H3</f>
-        <v>6.1201416720313743E-4</v>
+        <v>6.0499999994202442E-4</v>
       </c>
       <c r="J3" s="117" t="b">
         <f>NOT(ISERROR(I3))</f>
@@ -8236,11 +8234,11 @@
       </c>
       <c r="K3" s="119">
         <f>K4</f>
-        <v>-7.163187341494072E-8</v>
+        <v>-5.3786613586453301E-7</v>
       </c>
       <c r="L3" s="108">
         <f>_xll.ohFilter($I$2:$I$3,$J$2:$J$3)-K3*_xll.ohFilter($P$2:$P$3,$J$2:$J$3)</f>
-        <v>6.143063871524155E-4</v>
+        <v>6.2274958242555399E-4</v>
       </c>
       <c r="M3" s="118"/>
       <c r="N3" s="120">
@@ -8249,20 +8247,20 @@
       </c>
       <c r="O3" s="120">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P3" s="120">
         <f>(O3^2-N3^2)/(O3-N3)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="117"/>
       <c r="R3" s="131">
         <f>(O3^3-N3^3)/3/(O3-N3)</f>
-        <v>341.33333333333331</v>
+        <v>363</v>
       </c>
       <c r="S3" s="131">
         <f>(O3+N3)/2</f>
-        <v>16</v>
+        <v>16.5</v>
       </c>
       <c r="T3" s="131">
         <v>1</v>
@@ -8275,7 +8273,7 @@
       </c>
       <c r="B4" s="65" t="str">
         <f>_xll.qlMakeDatedOIS(,E4,F4,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00289#0000</v>
+        <v>obj_00490#0000</v>
       </c>
       <c r="C4" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B4,OisEngine)</f>
@@ -8286,23 +8284,23 @@
       </c>
       <c r="E4" s="55">
         <f>F3</f>
-        <v>41786</v>
+        <v>41799</v>
       </c>
       <c r="F4" s="56">
         <f>F5</f>
-        <v>41815</v>
+        <v>41827</v>
       </c>
       <c r="G4" s="27">
         <f>((1+G5*(F5-E5)/360)/(1+G3*(F3-E3)/360)-1)/(F4-E4)*360</f>
-        <v>1.5375159924341816E-3</v>
+        <v>1.5156837559380876E-3</v>
       </c>
       <c r="H4" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B4,_xll.ohTrigger(C4,InterestRatesTrigger))</f>
-        <v>9.298713695093556E-4</v>
+        <v>9.4349359028379971E-4</v>
       </c>
       <c r="I4" s="16">
         <f>G4-H4</f>
-        <v>6.0764462292482605E-4</v>
+        <v>5.721901656542879E-4</v>
       </c>
       <c r="J4" s="1" t="b">
         <f>NOT(ISERROR(I4))</f>
@@ -8310,16 +8308,16 @@
       </c>
       <c r="K4" s="15">
         <f>(I4-_xll.ohFilter($I$2:$I$3,$J$2:$J$3))/(P4-_xll.ohFilter($P$2:$P$3,$J$2:$J$3))</f>
-        <v>-7.163187341494072E-8</v>
+        <v>-5.3786613586453301E-7</v>
       </c>
       <c r="L4" s="15">
         <f>_xll.ohFilter($I$2:$I$3,$J$2:$J$3)-K4*_xll.ohFilter($P$2:$P$3,$J$2:$J$3)</f>
-        <v>6.143063871524155E-4</v>
+        <v>6.2274958242555399E-4</v>
       </c>
       <c r="M4" s="5"/>
       <c r="N4" s="121">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O4" s="121">
         <f t="shared" si="0"/>
@@ -8327,15 +8325,15 @@
       </c>
       <c r="P4" s="121">
         <f>(O4^2-N4^2)/(O4-N4)</f>
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="R4" s="100">
         <f>(O4^3-N4^3)/3/(O4-N4)</f>
-        <v>2232.333333333333</v>
+        <v>2274.3333333333335</v>
       </c>
       <c r="S4" s="100">
         <f>(O4+N4)/2</f>
-        <v>46.5</v>
+        <v>47</v>
       </c>
       <c r="T4" s="100">
         <v>1</v>
@@ -8351,15 +8349,15 @@
       </c>
       <c r="E5" s="55">
         <f>SettlementDate</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="F5" s="56">
         <f>_xll.qlCalendarAdvance(Calendar,E5,"2M","mf")</f>
-        <v>41815</v>
+        <v>41827</v>
       </c>
       <c r="G5" s="52">
         <f>_xll.qlQuoteValue(D5,AllTriggers)</f>
-        <v>1.5299999999999999E-3</v>
+        <v>1.5100000000000001E-3</v>
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="16"/>
@@ -8382,7 +8380,7 @@
       </c>
       <c r="B6" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E6,F6,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00282#0000</v>
+        <v>obj_00489#0000</v>
       </c>
       <c r="C6" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B6,OisEngine)</f>
@@ -8394,23 +8392,23 @@
       </c>
       <c r="E6" s="112">
         <f>SettlementDate</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="F6" s="113">
         <f>_xll.qlCalendarAdvance(Calendar,E6,A7,"mf")</f>
-        <v>41845</v>
+        <v>41858</v>
       </c>
       <c r="G6" s="114">
         <f>_xll.qlQuoteValue(D6,AllTriggers)</f>
-        <v>2.2875E-3</v>
+        <v>2.2285E-3</v>
       </c>
       <c r="H6" s="115">
         <f>_xll.qlOvernightIndexedSwapFairRate(B6,_xll.ohTrigger(C6,InterestRatesTrigger))</f>
-        <v>9.200000000000538E-4</v>
+        <v>9.2999999946704562E-4</v>
       </c>
       <c r="I6" s="116">
         <f t="shared" si="1"/>
-        <v>1.3674999999999462E-3</v>
+        <v>1.2985000005329545E-3</v>
       </c>
       <c r="J6" s="117" t="b">
         <v>0</v>
@@ -8424,33 +8422,33 @@
       </c>
       <c r="O6" s="120">
         <f t="shared" ref="O6:O27" si="3">F6-SettlementDate</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P6" s="120">
         <f>(O6^2-N6^2)/(O6-N6)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q6" s="117"/>
       <c r="R6" s="131">
         <f t="shared" ref="R6:R14" si="4">(O6^3-N6^3)/3/(O6-N6)</f>
-        <v>2760.3333333333335</v>
+        <v>2821.333333333333</v>
       </c>
       <c r="S6" s="131">
         <f t="shared" ref="S6:S14" si="5">(O6+N6)/2</f>
-        <v>45.5</v>
+        <v>46</v>
       </c>
       <c r="T6" s="131">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A7" s="238" t="str">
+      <c r="A7" s="232" t="str">
         <f>_xll.qlPeriodEquivalent(A6&amp;"M")</f>
         <v>3M</v>
       </c>
       <c r="B7" s="65" t="str">
         <f>_xll.qlMakeDatedOIS(,E7,F7,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00288#0000</v>
+        <v>obj_0048f#0000</v>
       </c>
       <c r="C7" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B7,OisEngine)</f>
@@ -8462,23 +8460,23 @@
       </c>
       <c r="E7" s="105">
         <f>E6</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="F7" s="106">
         <f>F6</f>
-        <v>41845</v>
+        <v>41858</v>
       </c>
       <c r="G7" s="107">
         <f>_xll.qlQuoteValue(D7,AllTriggers)</f>
-        <v>2.2875E-3</v>
+        <v>2.2285E-3</v>
       </c>
       <c r="H7" s="108">
         <f>_xll.qlOvernightIndexedSwapFairRate(B7,_xll.ohTrigger(C7,InterestRatesTrigger))</f>
-        <v>9.200000000000538E-4</v>
+        <v>9.2999999946704562E-4</v>
       </c>
       <c r="I7" s="109">
         <f t="shared" si="1"/>
-        <v>1.3674999999999462E-3</v>
+        <v>1.2985000005329545E-3</v>
       </c>
       <c r="J7" s="117" t="b">
         <f>AND(ISERROR(I8),ISERROR(I9),NOT(ISERROR(I7)))</f>
@@ -8493,27 +8491,27 @@
       </c>
       <c r="O7" s="120">
         <f t="shared" si="3"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="P7" s="120">
         <f t="shared" ref="P7:P14" si="6">(O7^2-N7^2)/(O7-N7)</f>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="Q7" s="117"/>
       <c r="R7" s="131">
         <f t="shared" si="4"/>
-        <v>2760.3333333333335</v>
+        <v>2821.333333333333</v>
       </c>
       <c r="S7" s="131">
         <f t="shared" si="5"/>
-        <v>45.5</v>
+        <v>46</v>
       </c>
       <c r="T7" s="131">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A8" s="238" t="str">
+      <c r="A8" s="232" t="str">
         <f>PROPER(Currency)&amp;IborType&amp;A7</f>
         <v>UsdLibor3M</v>
       </c>
@@ -8537,11 +8535,11 @@
       <c r="M8" s="118"/>
       <c r="N8" s="120">
         <f t="shared" si="2"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="O8" s="120">
         <f t="shared" si="3"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="P8" s="120" t="e">
         <f t="shared" si="6"/>
@@ -8554,7 +8552,7 @@
       </c>
       <c r="S8" s="131">
         <f t="shared" si="5"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="T8" s="131">
         <v>1</v>
@@ -8585,20 +8583,20 @@
       </c>
       <c r="K9" s="108">
         <f>AVERAGE(_xll.ohFilter(K10:K12,J10:J12))</f>
-        <v>-3.7175264097954424E-7</v>
+        <v>-8.0180558696483716E-7</v>
       </c>
       <c r="L9" s="108">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K9*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>1.4013294903290848E-3</v>
+        <v>1.3722661145337196E-3</v>
       </c>
       <c r="M9" s="118"/>
       <c r="N9" s="120">
         <f t="shared" si="2"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="O9" s="120">
         <f t="shared" si="3"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="P9" s="120" t="e">
         <f t="shared" si="6"/>
@@ -8611,18 +8609,18 @@
       </c>
       <c r="S9" s="131">
         <f t="shared" si="5"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="T9" s="131">
         <v>1</v>
       </c>
       <c r="V9" s="91">
         <f t="array" ref="V9:V11">_xll.ohFilter(R6:R14,$J6:$J14)</f>
-        <v>2760.3333333333335</v>
+        <v>2821.333333333333</v>
       </c>
       <c r="W9" s="92">
         <f t="array" ref="W9:W11">_xll.ohFilter(S6:S14,$J6:$J14)</f>
-        <v>45.5</v>
+        <v>46</v>
       </c>
       <c r="X9" s="93">
         <f t="array" ref="X9:X11">_xll.ohFilter(T6:T14,$J6:$J14)</f>
@@ -8630,35 +8628,35 @@
       </c>
       <c r="Z9" s="76">
         <f t="array" ref="Z9:Z11">MMULT(AD9:AF11,AB9:AB11)</f>
-        <v>2.4255205846153995E-8</v>
+        <v>3.1587917154378896E-8</v>
       </c>
       <c r="AB9" s="76">
         <f t="array" ref="AB9:AB11">_xll.ohFilter(I6:I14,$J6:$J14)</f>
-        <v>1.3674999999999462E-3</v>
+        <v>1.2985000005329545E-3</v>
       </c>
       <c r="AD9" s="82">
         <f t="array" ref="AD9:AF11">MINVERSE(V9:X11)</f>
-        <v>6.9979006298110584E-4</v>
+        <v>1.7006802721088478E-3</v>
       </c>
       <c r="AE9" s="83">
-        <v>-1.3620913725882239E-3</v>
+        <v>-2.5510204081632716E-3</v>
       </c>
       <c r="AF9" s="84">
-        <v>6.6230130960711784E-4</v>
+        <v>8.5034013605442401E-4</v>
       </c>
       <c r="AH9" s="79">
         <f t="array" ref="AH9:AH11">MMULT(V9:X11,Z9:Z11)-AB9:AB11</f>
-        <v>8.6736173798840355E-19</v>
+        <v>2.1684043449710089E-18</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A10" s="238" t="str">
+      <c r="A10" s="232" t="str">
         <f>_xll.qlIMMNextCode(EvaluationDate,FALSE)</f>
         <v>K4</v>
       </c>
       <c r="B10" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E10,F10,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0032d#0000</v>
+        <v>obj_00487#0000</v>
       </c>
       <c r="C10" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B10,OisEngine)</f>
@@ -8678,15 +8676,15 @@
       </c>
       <c r="G10" s="52">
         <f>1-_xll.qlQuoteValue($D10,AllTriggers)/100</f>
-        <v>2.2874999999999979E-3</v>
+        <v>2.2124999999999506E-3</v>
       </c>
       <c r="H10" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B10,_xll.ohTrigger(C10,InterestRatesTrigger))</f>
-        <v>9.4652137208311765E-4</v>
+        <v>9.4385006975855851E-4</v>
       </c>
       <c r="I10" s="16">
         <f t="shared" si="1"/>
-        <v>1.3409786279168802E-3</v>
+        <v>1.2686499302413921E-3</v>
       </c>
       <c r="J10" s="1" t="b">
         <f>AND(NOT(ISERROR(I10)),E10&lt;&gt;$E$9,E10&lt;&gt;$E$8)</f>
@@ -8694,41 +8692,41 @@
       </c>
       <c r="K10" s="15">
         <f>(I10-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P10-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>-5.0040324685030221E-7</v>
+        <v>-1.066073938984371E-6</v>
       </c>
       <c r="L10" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K10*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>1.4130366954633238E-3</v>
+        <v>1.3965788029195166E-3</v>
       </c>
       <c r="M10" s="5"/>
       <c r="N10" s="121">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="O10" s="121">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="P10" s="121">
         <f t="shared" si="6"/>
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="R10" s="100">
         <f t="shared" si="4"/>
-        <v>5889.333333333333</v>
+        <v>4305.3333333333339</v>
       </c>
       <c r="S10" s="100">
         <f t="shared" si="5"/>
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="T10" s="100">
         <v>1</v>
       </c>
       <c r="V10" s="94">
-        <v>5889.333333333333</v>
+        <v>4305.3333333333339</v>
       </c>
       <c r="W10" s="95">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="X10" s="96">
         <v>1</v>
@@ -8737,35 +8735,35 @@
         <v>47</v>
       </c>
       <c r="Z10" s="77">
-        <v>-3.8647513651200672E-6</v>
+        <v>-5.4804670963328801E-6</v>
       </c>
       <c r="AA10" s="67" t="s">
         <v>48</v>
       </c>
       <c r="AB10" s="77">
-        <v>1.3409786279168802E-3</v>
+        <v>1.2686499302413921E-3</v>
       </c>
       <c r="AD10" s="85">
-        <v>-0.12036389083275019</v>
+        <v>-0.2517006802721094</v>
       </c>
       <c r="AE10" s="86">
-        <v>0.19856543037088875</v>
+        <v>0.34183673469387837</v>
       </c>
       <c r="AF10" s="87">
-        <v>-7.8201539538138548E-2</v>
+        <v>-9.0136054421768988E-2</v>
       </c>
       <c r="AH10" s="80">
-        <v>8.6736173798840355E-19</v>
+        <v>2.3852447794681098E-18</v>
       </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A11" s="238" t="str">
+      <c r="A11" s="232" t="str">
         <f>_xll.qlIMMNextCode(E10,IF(_xll.qlIMMIsIMMdate(E10,TRUE),FALSE,TRUE))</f>
         <v>M4</v>
       </c>
       <c r="B11" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E11,F11,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0032c#0001</v>
+        <v>obj_00472#0000</v>
       </c>
       <c r="C11" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B11,OisEngine)</f>
@@ -8785,15 +8783,15 @@
       </c>
       <c r="G11" s="52">
         <f>1-_xll.qlQuoteValue($D11,AllTriggers)/100</f>
-        <v>2.3250000000000215E-3</v>
+        <v>2.2249999999999215E-3</v>
       </c>
       <c r="H11" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B11,_xll.ohTrigger(C11,InterestRatesTrigger))</f>
-        <v>9.7542133895142538E-4</v>
+        <v>9.7890281976810499E-4</v>
       </c>
       <c r="I11" s="16">
         <f t="shared" si="1"/>
-        <v>1.3495786610485962E-3</v>
+        <v>1.2460971802318165E-3</v>
       </c>
       <c r="J11" s="1" t="b">
         <f>NOT(ISERROR(I11))</f>
@@ -8801,62 +8799,62 @@
       </c>
       <c r="K11" s="15">
         <f>(I11-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P11-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>-1.644159536821102E-7</v>
+        <v>-6.2384309882307147E-7</v>
       </c>
       <c r="L11" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K11*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>1.3824618517850184E-3</v>
+        <v>1.355893565624677E-3</v>
       </c>
       <c r="M11" s="5"/>
       <c r="N11" s="121">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="O11" s="121">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="P11" s="121">
         <f t="shared" si="6"/>
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="R11" s="100">
         <f t="shared" si="4"/>
-        <v>10705.333333333332</v>
+        <v>8449.3333333333321</v>
       </c>
       <c r="S11" s="100">
         <f t="shared" si="5"/>
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="T11" s="100">
         <v>1</v>
       </c>
       <c r="V11" s="97">
-        <v>10705.333333333332</v>
+        <v>8449.3333333333321</v>
       </c>
       <c r="W11" s="98">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="X11" s="99">
         <v>1</v>
       </c>
       <c r="Z11" s="78">
-        <v>1.4763937339089097E-3</v>
+        <v>1.461481443366048E-3</v>
       </c>
       <c r="AB11" s="78">
-        <v>1.3495786610485962E-3</v>
+        <v>1.2460971802318165E-3</v>
       </c>
       <c r="AD11" s="88">
-        <v>4.5449031957079544</v>
+        <v>7.7800453514739374</v>
       </c>
       <c r="AE11" s="89">
-        <v>-5.2749008630744108</v>
+        <v>-8.527210884353762</v>
       </c>
       <c r="AF11" s="90">
-        <v>1.7299976673664565</v>
+        <v>1.7471655328798255</v>
       </c>
       <c r="AH11" s="81">
-        <v>6.5052130349130266E-19</v>
+        <v>3.4694469519536142E-18</v>
       </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
@@ -8865,7 +8863,7 @@
       </c>
       <c r="B12" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E12,F12,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0032e#0000</v>
+        <v>obj_00473#0000</v>
       </c>
       <c r="C12" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B12,OisEngine)</f>
@@ -8877,23 +8875,23 @@
       </c>
       <c r="E12" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A12&amp;"M","mf")</f>
-        <v>41786</v>
+        <v>41799</v>
       </c>
       <c r="F12" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$8,E12)</f>
-        <v>41878</v>
+        <v>41891</v>
       </c>
       <c r="G12" s="52">
         <f>_xll.qlQuoteValue(D12,AllTriggers)</f>
-        <v>2.2899999999999999E-3</v>
+        <v>2.2200000000000002E-3</v>
       </c>
       <c r="H12" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B12,_xll.ohTrigger(C12,InterestRatesTrigger))</f>
-        <v>9.5177851695645813E-4</v>
+        <v>9.6872298119079223E-4</v>
       </c>
       <c r="I12" s="16">
         <f>G12-H12</f>
-        <v>1.3382214830435419E-3</v>
+        <v>1.251277018809208E-3</v>
       </c>
       <c r="J12" s="1" t="b">
         <f>AND(NOT(ISERROR(I12)),E12&lt;&gt;$E$11,E12&lt;&gt;$E$10)</f>
@@ -8901,32 +8899,32 @@
       </c>
       <c r="K12" s="15">
         <f>(I12-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P12-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>-4.504387224062203E-7</v>
+        <v>-7.1549972308706887E-7</v>
       </c>
       <c r="L12" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K12*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>1.4084899237389124E-3</v>
+        <v>1.3643259750569649E-3</v>
       </c>
       <c r="M12" s="5"/>
       <c r="N12" s="121">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O12" s="121">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="P12" s="121">
         <f t="shared" si="6"/>
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="R12" s="100">
         <f t="shared" si="4"/>
-        <v>6789.333333333333</v>
+        <v>6946.333333333333</v>
       </c>
       <c r="S12" s="100">
         <f t="shared" si="5"/>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="T12" s="100">
         <v>1</v>
@@ -8941,7 +8939,7 @@
       </c>
       <c r="B13" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E13,F13,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0032f#0000</v>
+        <v>obj_00470#0000</v>
       </c>
       <c r="C13" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B13,OisEngine)</f>
@@ -8953,23 +8951,23 @@
       </c>
       <c r="E13" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A13&amp;"M","mf")</f>
-        <v>41815</v>
+        <v>41827</v>
       </c>
       <c r="F13" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$8,E13)</f>
-        <v>41907</v>
+        <v>41919</v>
       </c>
       <c r="G13" s="52">
         <f>_xll.qlQuoteValue(D13,AllTriggers)</f>
-        <v>2.3400000000000001E-3</v>
+        <v>2.2500000000000003E-3</v>
       </c>
       <c r="H13" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B13,_xll.ohTrigger(C13,InterestRatesTrigger))</f>
-        <v>9.8636797532269472E-4</v>
+        <v>1.0029958170922604E-3</v>
       </c>
       <c r="I13" s="16">
         <f>G13-H13</f>
-        <v>1.3536320246773054E-3</v>
+        <v>1.2470041829077399E-3</v>
       </c>
       <c r="J13" s="1" t="b">
         <f>AND(NOT(ISERROR(I13)),E13&lt;&gt;$E$11,E13&lt;&gt;$E$10)</f>
@@ -8977,11 +8975,11 @@
       </c>
       <c r="K13" s="15">
         <f>(I13-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P13-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>-1.1274776685073888E-7</v>
+        <v>-4.2209686578044786E-7</v>
       </c>
       <c r="L13" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K13*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>1.3777600467833634E-3</v>
+        <v>1.3373329121847558E-3</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="121">
@@ -9017,7 +9015,7 @@
       </c>
       <c r="B14" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E14,F14,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00330#0000</v>
+        <v>obj_00475#0000</v>
       </c>
       <c r="C14" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B14,OisEngine)</f>
@@ -9029,23 +9027,23 @@
       </c>
       <c r="E14" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A14&amp;"M","mf")</f>
-        <v>41845</v>
+        <v>41858</v>
       </c>
       <c r="F14" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$8,E14)</f>
-        <v>41939</v>
+        <v>41950</v>
       </c>
       <c r="G14" s="52">
         <f>_xll.qlQuoteValue(D14,AllTriggers)</f>
-        <v>2.3799999999999997E-3</v>
+        <v>2.2899999999999999E-3</v>
       </c>
       <c r="H14" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B14,_xll.ohTrigger(C14,InterestRatesTrigger))</f>
-        <v>1.0575200252880845E-3</v>
+        <v>1.0697457576254274E-3</v>
       </c>
       <c r="I14" s="16">
         <f>G14-H14</f>
-        <v>1.3224799747119152E-3</v>
+        <v>1.2202542423745725E-3</v>
       </c>
       <c r="J14" s="1" t="b">
         <f>AND(NOT(ISERROR(I14)),E14&lt;&gt;$E$11,E14&lt;&gt;$E$10)</f>
@@ -9053,20 +9051,20 @@
       </c>
       <c r="K14" s="15">
         <f>(I14-_xll.ohFilter($I$6:$I$9,$J$6:$J$9))/(P14-_xll.ohFilter($P$6:$P$9,$J$6:$J$9))</f>
-        <v>-2.4335148804341083E-7</v>
+        <v>-4.2524868564338047E-7</v>
       </c>
       <c r="L14" s="15">
         <f>_xll.ohFilter($I$6:$I$9,$J$6:$J$9)-K14*_xll.ohFilter($P$6:$P$9,$J$6:$J$9)</f>
-        <v>1.3896449854118966E-3</v>
+        <v>1.3376228796121454E-3</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="121">
         <f t="shared" si="2"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O14" s="121">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P14" s="121">
         <f t="shared" si="6"/>
@@ -9074,7 +9072,7 @@
       </c>
       <c r="R14" s="100">
         <f t="shared" si="4"/>
-        <v>19780.333333333332</v>
+        <v>19749.333333333336</v>
       </c>
       <c r="S14" s="100">
         <f t="shared" si="5"/>
@@ -9093,7 +9091,7 @@
       </c>
       <c r="B15" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E15,F15,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00333#0000</v>
+        <v>obj_00474#0000</v>
       </c>
       <c r="C15" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B15,OisEngine)</f>
@@ -9105,23 +9103,23 @@
       </c>
       <c r="E15" s="112">
         <f>SettlementDate</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="F15" s="113">
         <f>_xll.qlCalendarAdvance(Calendar,E15,A16,"mf")</f>
-        <v>41939</v>
+        <v>41950</v>
       </c>
       <c r="G15" s="114">
         <f>_xll.qlQuoteValue($D15,AllTriggers)</f>
-        <v>3.228E-3</v>
+        <v>3.2200000000000002E-3</v>
       </c>
       <c r="H15" s="115">
         <f>_xll.qlOvernightIndexedSwapFairRate(B15,_xll.ohTrigger(C15,InterestRatesTrigger))</f>
-        <v>9.8999999999881626E-4</v>
+        <v>1.0000000000004693E-3</v>
       </c>
       <c r="I15" s="116">
         <f t="shared" si="1"/>
-        <v>2.2380000000011835E-3</v>
+        <v>2.2199999999995309E-3</v>
       </c>
       <c r="J15" s="117" t="b">
         <v>0</v>
@@ -9135,33 +9133,33 @@
       </c>
       <c r="O15" s="120">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P15" s="120">
         <f t="shared" ref="P15:P27" si="7">(O15^2-N15^2)/(O15-N15)</f>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q15" s="117"/>
       <c r="R15" s="131">
         <f t="shared" ref="R15:R27" si="8">(O15^3-N15^3)/3/(O15-N15)</f>
-        <v>11408.333333333332</v>
+        <v>11285.333333333332</v>
       </c>
       <c r="S15" s="131">
         <f t="shared" ref="S15:S27" si="9">(O15+N15)/2</f>
-        <v>92.5</v>
+        <v>92</v>
       </c>
       <c r="T15" s="131">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A16" s="238" t="str">
+      <c r="A16" s="232" t="str">
         <f>_xll.qlPeriodEquivalent(A15&amp;"M")</f>
         <v>6M</v>
       </c>
       <c r="B16" s="65" t="str">
         <f>_xll.qlMakeDatedOIS(,E16,F16,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00332#0001</v>
+        <v>obj_0048d#0000</v>
       </c>
       <c r="C16" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B16,OisEngine)</f>
@@ -9173,23 +9171,23 @@
       </c>
       <c r="E16" s="105">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlLastFixingQuoteReferenceDate(D16),_xll.qlInterestRateIndexFixingDays(A17)&amp;"D","f",,LastFixingsTrigger)</f>
-        <v>41754</v>
+        <v>41765</v>
       </c>
       <c r="F16" s="106">
         <f>_xll.qlInterestRateIndexMaturity(A17,E16)</f>
-        <v>41939</v>
+        <v>41949</v>
       </c>
       <c r="G16" s="107">
         <f>_xll.qlQuoteValue(D16,AllTriggers)</f>
-        <v>3.228E-3</v>
+        <v>3.2200000000000002E-3</v>
       </c>
       <c r="H16" s="108">
         <f>_xll.qlOvernightIndexedSwapFairRate(B16,_xll.ohTrigger(C16,InterestRatesTrigger))</f>
-        <v>9.8999999999881626E-4</v>
+        <v>1.0017321044090675E-3</v>
       </c>
       <c r="I16" s="109">
         <f t="shared" si="1"/>
-        <v>2.2380000000011835E-3</v>
+        <v>2.2182678955909325E-3</v>
       </c>
       <c r="J16" s="117" t="b">
         <f>AND(ISERROR(I17),ISERROR(I18),NOT(ISERROR(I16)))</f>
@@ -9200,31 +9198,31 @@
       <c r="M16" s="118"/>
       <c r="N16" s="120">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O16" s="120">
         <f t="shared" si="3"/>
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="P16" s="120">
         <f t="shared" si="7"/>
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q16" s="117"/>
       <c r="R16" s="131">
         <f t="shared" si="8"/>
-        <v>11408.333333333332</v>
+        <v>11102.333333333332</v>
       </c>
       <c r="S16" s="131">
         <f t="shared" si="9"/>
-        <v>92.5</v>
+        <v>91</v>
       </c>
       <c r="T16" s="131">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A17" s="238" t="str">
+      <c r="A17" s="232" t="str">
         <f>PROPER(Currency)&amp;IborType&amp;A16</f>
         <v>UsdLibor6M</v>
       </c>
@@ -9248,11 +9246,11 @@
       <c r="M17" s="118"/>
       <c r="N17" s="120">
         <f t="shared" si="2"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="O17" s="120">
         <f t="shared" si="3"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="P17" s="120" t="e">
         <f t="shared" si="7"/>
@@ -9265,7 +9263,7 @@
       </c>
       <c r="S17" s="131">
         <f t="shared" si="9"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="T17" s="131">
         <v>1</v>
@@ -9296,20 +9294,20 @@
       </c>
       <c r="K18" s="108">
         <f>AVERAGE(_xll.ohFilter(K19:K21,J19:J21))</f>
-        <v>-2.6339997809853552E-7</v>
+        <v>-5.814751652831254E-7</v>
       </c>
       <c r="L18" s="108">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K18*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>2.2867289959494124E-3</v>
+        <v>2.3240963756724613E-3</v>
       </c>
       <c r="M18" s="118"/>
       <c r="N18" s="120">
         <f t="shared" si="2"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="O18" s="120">
         <f t="shared" si="3"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="P18" s="120" t="e">
         <f t="shared" si="7"/>
@@ -9322,18 +9320,18 @@
       </c>
       <c r="S18" s="131">
         <f t="shared" si="9"/>
-        <v>-41754</v>
+        <v>-41766</v>
       </c>
       <c r="T18" s="131">
         <v>1</v>
       </c>
       <c r="V18" s="91">
         <f t="array" ref="V18:V20">_xll.ohFilter(R15:R24,$J15:$J24)</f>
-        <v>11408.333333333332</v>
+        <v>11102.333333333332</v>
       </c>
       <c r="W18" s="92">
         <f t="array" ref="W18:W20">_xll.ohFilter(S15:S24,$J15:$J24)</f>
-        <v>92.5</v>
+        <v>91</v>
       </c>
       <c r="X18" s="93">
         <f t="array" ref="X18:X20">_xll.ohFilter(T15:T24,$J15:$J24)</f>
@@ -9341,25 +9339,25 @@
       </c>
       <c r="Z18" s="76">
         <f t="array" ref="Z18:Z20">MMULT(AD18:AF20,AB18:AB20)</f>
-        <v>2.0400485387877149E-8</v>
+        <v>1.8183142703755349E-8</v>
       </c>
       <c r="AB18" s="76">
         <f t="array" ref="AB18:AB20">_xll.ohFilter(I15:I24,$J15:$J24)</f>
-        <v>2.2380000000011835E-3</v>
+        <v>2.2182678955909325E-3</v>
       </c>
       <c r="AD18" s="82">
         <f t="array" ref="AD18:AF20">MINVERSE(V18:X20)</f>
-        <v>4.8777315296566059E-4</v>
+        <v>4.6651970841154181E-4</v>
       </c>
       <c r="AE18" s="83">
-        <v>-1.0080645161290318E-3</v>
+        <v>-1.0148849797023017E-3</v>
       </c>
       <c r="AF18" s="84">
-        <v>5.2029136316337132E-4</v>
+        <v>5.4836527129075992E-4</v>
       </c>
       <c r="AH18" s="79">
         <f t="array" ref="AH18:AH20">MMULT(V18:X20,Z18:Z20)-AB18:AB20</f>
-        <v>4.3368086899420177E-18</v>
+        <v>-1.7347234759768071E-18</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
@@ -9368,56 +9366,56 @@
       </c>
       <c r="B19" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E19,F19,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00334#0000</v>
+        <v>obj_00482#0000</v>
       </c>
       <c r="C19" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B19,OisEngine)</f>
         <v>1</v>
       </c>
       <c r="D19" s="11" t="str">
-        <f>Currency&amp;A19&amp;"x"&amp;A19+6&amp;"F"&amp;QuoteSuffix</f>
+        <f t="shared" ref="D19:D24" si="10">Currency&amp;A19&amp;"x"&amp;A19+6&amp;"F"&amp;QuoteSuffix</f>
         <v>USD1x7F_Quote</v>
       </c>
       <c r="E19" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A19&amp;"M","mf")</f>
-        <v>41786</v>
+        <v>41799</v>
       </c>
       <c r="F19" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E19)</f>
-        <v>41971</v>
+        <v>41982</v>
       </c>
       <c r="G19" s="27">
         <f>_xll.qlQuoteValue(D19,AllTriggers)</f>
-        <v>3.2499999999999994E-3</v>
+        <v>3.2199999999999993E-3</v>
       </c>
       <c r="H19" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B19,_xll.ohTrigger(C19,InterestRatesTrigger))</f>
-        <v>1.0409991832463117E-3</v>
+        <v>1.0545039539739298E-3</v>
       </c>
       <c r="I19" s="16">
-        <f t="shared" ref="I19:I24" si="10">G19-H19</f>
-        <v>2.2090008167536877E-3</v>
+        <f t="shared" ref="I19:I24" si="11">G19-H19</f>
+        <v>2.1654960460260695E-3</v>
       </c>
       <c r="J19" s="1" t="b">
-        <f t="shared" ref="J19:J24" si="11">NOT(ISERROR(I19))</f>
+        <f t="shared" ref="J19:J24" si="12">NOT(ISERROR(I19))</f>
         <v>1</v>
       </c>
       <c r="K19" s="15">
         <f>(I19-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P19-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-4.5311223824212149E-7</v>
+        <v>-7.8763954574422344E-7</v>
       </c>
       <c r="L19" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K19*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>2.3218257640759761E-3</v>
+        <v>2.361618292916381E-3</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="121">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O19" s="121">
         <f t="shared" si="3"/>
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P19" s="121">
         <f t="shared" si="7"/>
@@ -9425,7 +9423,7 @@
       </c>
       <c r="R19" s="100">
         <f t="shared" si="8"/>
-        <v>18352.333333333332</v>
+        <v>18291</v>
       </c>
       <c r="S19" s="100">
         <f t="shared" si="9"/>
@@ -9435,7 +9433,7 @@
         <v>1</v>
       </c>
       <c r="V19" s="94">
-        <v>18352.333333333332</v>
+        <v>18291</v>
       </c>
       <c r="W19" s="95">
         <v>124.5</v>
@@ -9447,25 +9445,25 @@
         <v>47</v>
       </c>
       <c r="Z19" s="77">
-        <v>-5.3331298056535285E-6</v>
+        <v>-5.4771463108833191E-6</v>
       </c>
       <c r="AA19" s="67" t="s">
         <v>48</v>
       </c>
       <c r="AB19" s="77">
-        <v>2.2090008167536877E-3</v>
+        <v>2.1654960460260695E-3</v>
       </c>
       <c r="AD19" s="85">
-        <v>-0.13709677419354835</v>
+        <v>-0.1299598411104807</v>
       </c>
       <c r="AE19" s="86">
-        <v>0.24999999999999989</v>
+        <v>0.24763193504736158</v>
       </c>
       <c r="AF19" s="87">
-        <v>-0.11290322580645157</v>
+        <v>-0.1176720939368809</v>
       </c>
       <c r="AH19" s="80">
-        <v>6.0715321659188248E-18</v>
+        <v>-8.6736173798840355E-19</v>
       </c>
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.2">
@@ -9474,47 +9472,47 @@
       </c>
       <c r="B20" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E20,F20,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00337#0000</v>
+        <v>obj_0048a#0000</v>
       </c>
       <c r="C20" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B20,OisEngine)</f>
         <v>1</v>
       </c>
       <c r="D20" s="11" t="str">
-        <f>Currency&amp;A20&amp;"x"&amp;A20+6&amp;"F"&amp;QuoteSuffix</f>
+        <f t="shared" si="10"/>
         <v>USD2x8F_Quote</v>
       </c>
       <c r="E20" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A20&amp;"M","mf")</f>
-        <v>41815</v>
+        <v>41827</v>
       </c>
       <c r="F20" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E20)</f>
-        <v>42002</v>
+        <v>42011</v>
       </c>
       <c r="G20" s="27">
         <f>_xll.qlQuoteValue(D20,AllTriggers)</f>
-        <v>3.2999999999999995E-3</v>
+        <v>3.2599999999999994E-3</v>
       </c>
       <c r="H20" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B20,_xll.ohTrigger(C20,InterestRatesTrigger))</f>
-        <v>1.0789761846253399E-3</v>
+        <v>1.1062405928614241E-3</v>
       </c>
       <c r="I20" s="16">
-        <f t="shared" si="10"/>
-        <v>2.2210238153746596E-3</v>
+        <f t="shared" si="11"/>
+        <v>2.1537594071385753E-3</v>
       </c>
       <c r="J20" s="1" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K20" s="15">
         <f>(I20-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P20-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-1.3690471473003103E-7</v>
+        <v>-5.2022974558352525E-7</v>
       </c>
       <c r="L20" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K20*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>2.2633273722262393E-3</v>
+        <v>2.3129497092871341E-3</v>
       </c>
       <c r="M20" s="5"/>
       <c r="N20" s="121">
@@ -9523,49 +9521,49 @@
       </c>
       <c r="O20" s="121">
         <f t="shared" si="3"/>
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="P20" s="121">
         <f t="shared" si="7"/>
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="R20" s="100">
         <f t="shared" si="8"/>
-        <v>26784.333333333332</v>
+        <v>26230.333333333332</v>
       </c>
       <c r="S20" s="100">
         <f t="shared" si="9"/>
-        <v>154.5</v>
+        <v>153</v>
       </c>
       <c r="T20" s="100">
         <v>1</v>
       </c>
       <c r="V20" s="97">
-        <v>26784.333333333332</v>
+        <v>26230.333333333332</v>
       </c>
       <c r="W20" s="98">
-        <v>154.5</v>
+        <v>153</v>
       </c>
       <c r="X20" s="99">
         <v>1</v>
       </c>
       <c r="Z20" s="78">
-        <v>2.4985789695574408E-3</v>
+        <v>2.514812898536653E-3</v>
       </c>
       <c r="AB20" s="78">
-        <v>2.2210238153746596E-3</v>
+        <v>2.1537594071385753E-3</v>
       </c>
       <c r="AD20" s="88">
-        <v>8.1167728928199789</v>
+        <v>7.6468882316993367</v>
       </c>
       <c r="AE20" s="89">
-        <v>-11.624663978494622</v>
+        <v>-11.266914749661719</v>
       </c>
       <c r="AF20" s="90">
-        <v>4.5078910856746441</v>
+        <v>4.6200265179623816</v>
       </c>
       <c r="AH20" s="81">
-        <v>8.2399365108898337E-18</v>
+        <v>4.3368086899420177E-19</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.2">
@@ -9574,68 +9572,68 @@
       </c>
       <c r="B21" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E21,F21,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00336#0000</v>
+        <v>obj_00486#0000</v>
       </c>
       <c r="C21" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B21,OisEngine)</f>
         <v>1</v>
       </c>
       <c r="D21" s="11" t="str">
-        <f>Currency&amp;A21&amp;"x"&amp;A21+6&amp;"F"&amp;QuoteSuffix</f>
+        <f t="shared" si="10"/>
         <v>USD3x9F_Quote</v>
       </c>
       <c r="E21" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A21&amp;"M","mf")</f>
-        <v>41845</v>
+        <v>41858</v>
       </c>
       <c r="F21" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E21)</f>
-        <v>42030</v>
+        <v>42044</v>
       </c>
       <c r="G21" s="27">
         <f>_xll.qlQuoteValue(D21,AllTriggers)</f>
-        <v>3.3599999999999997E-3</v>
+        <v>3.3199999999999996E-3</v>
       </c>
       <c r="H21" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B21,_xll.ohTrigger(C21,InterestRatesTrigger))</f>
-        <v>1.1584333025996851E-3</v>
+        <v>1.1838046708591331E-3</v>
       </c>
       <c r="I21" s="16">
-        <f t="shared" si="10"/>
-        <v>2.2015666974003149E-3</v>
+        <f t="shared" si="11"/>
+        <v>2.1361953291408665E-3</v>
       </c>
       <c r="J21" s="1" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K21" s="15">
         <f>(I21-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P21-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-2.0018298132345395E-7</v>
+        <v>-4.3655620452162754E-7</v>
       </c>
       <c r="L21" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K21*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>2.2750338515460226E-3</v>
+        <v>2.2977211248138688E-3</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="121">
         <f t="shared" si="2"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O21" s="121">
         <f t="shared" si="3"/>
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="P21" s="121">
         <f t="shared" si="7"/>
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="R21" s="100">
         <f t="shared" si="8"/>
-        <v>36524.333333333336</v>
+        <v>37108</v>
       </c>
       <c r="S21" s="100">
         <f t="shared" si="9"/>
-        <v>183.5</v>
+        <v>185</v>
       </c>
       <c r="T21" s="100">
         <v>1</v>
@@ -9651,56 +9649,56 @@
       </c>
       <c r="B22" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E22,F22,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00339#0000</v>
+        <v>obj_00480#0000</v>
       </c>
       <c r="C22" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B22,OisEngine)</f>
         <v>1</v>
       </c>
       <c r="D22" s="11" t="str">
-        <f>Currency&amp;A22&amp;"x"&amp;A22+6&amp;"F"&amp;QuoteSuffix</f>
+        <f t="shared" si="10"/>
         <v>USD4x10F_Quote</v>
       </c>
       <c r="E22" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A22&amp;"M","mf")</f>
-        <v>41877</v>
+        <v>41890</v>
       </c>
       <c r="F22" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E22)</f>
-        <v>42061</v>
+        <v>42072</v>
       </c>
       <c r="G22" s="27">
         <f>_xll.qlQuoteValue(D22,AllTriggers)</f>
-        <v>3.4499999999999999E-3</v>
+        <v>3.4299999999999999E-3</v>
       </c>
       <c r="H22" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B22,_xll.ohTrigger(C22,InterestRatesTrigger))</f>
-        <v>1.2586773629802673E-3</v>
+        <v>1.2858429796138568E-3</v>
       </c>
       <c r="I22" s="16">
-        <f t="shared" si="10"/>
-        <v>2.1913226370197329E-3</v>
+        <f t="shared" si="11"/>
+        <v>2.1441570203861431E-3</v>
       </c>
       <c r="J22" s="1" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K22" s="15">
         <f>(I22-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P22-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-1.9051984890388013E-7</v>
+        <v>-2.9883417421286026E-7</v>
       </c>
       <c r="L22" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K22*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>2.2732461720484012E-3</v>
+        <v>2.2726557152976733E-3</v>
       </c>
       <c r="M22" s="5"/>
       <c r="N22" s="121">
         <f t="shared" si="2"/>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O22" s="121">
         <f t="shared" si="3"/>
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="P22" s="121">
         <f t="shared" si="7"/>
@@ -9708,7 +9706,7 @@
       </c>
       <c r="R22" s="100">
         <f t="shared" si="8"/>
-        <v>49046.333333333336</v>
+        <v>48985.333333333328</v>
       </c>
       <c r="S22" s="100">
         <f t="shared" si="9"/>
@@ -9728,47 +9726,47 @@
       </c>
       <c r="B23" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E23,F23,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00335#0000</v>
+        <v>obj_0047e#0000</v>
       </c>
       <c r="C23" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B23,OisEngine)</f>
         <v>1</v>
       </c>
       <c r="D23" s="11" t="str">
-        <f>Currency&amp;A23&amp;"x"&amp;A23+6&amp;"F"&amp;QuoteSuffix</f>
+        <f t="shared" si="10"/>
         <v>USD5x11F_Quote</v>
       </c>
       <c r="E23" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A23&amp;"M","mf")</f>
-        <v>41907</v>
+        <v>41919</v>
       </c>
       <c r="F23" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E23)</f>
-        <v>42088</v>
+        <v>42101</v>
       </c>
       <c r="G23" s="27">
         <f>_xll.qlQuoteValue(D23,AllTriggers)</f>
-        <v>3.5699999999999998E-3</v>
+        <v>3.5799999999999998E-3</v>
       </c>
       <c r="H23" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B23,_xll.ohTrigger(C23,InterestRatesTrigger))</f>
-        <v>1.3469642507371027E-3</v>
+        <v>1.411176484716123E-3</v>
       </c>
       <c r="I23" s="16">
-        <f t="shared" si="10"/>
-        <v>2.2230357492628973E-3</v>
+        <f t="shared" si="11"/>
+        <v>2.1688235152838766E-3</v>
       </c>
       <c r="J23" s="1" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K23" s="15">
         <f>(I23-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P23-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-4.9550499133397883E-8</v>
+        <v>-1.6158294217992113E-7</v>
       </c>
       <c r="L23" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K23*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>2.2471668423408621E-3</v>
+        <v>2.2476759910676782E-3</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="121">
@@ -9777,19 +9775,19 @@
       </c>
       <c r="O23" s="121">
         <f t="shared" si="3"/>
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="P23" s="121">
         <f t="shared" si="7"/>
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="R23" s="100">
         <f t="shared" si="8"/>
-        <v>62022.333333333336</v>
+        <v>62296.333333333328</v>
       </c>
       <c r="S23" s="100">
         <f t="shared" si="9"/>
-        <v>243.5</v>
+        <v>244</v>
       </c>
       <c r="T23" s="100">
         <v>1</v>
@@ -9805,68 +9803,68 @@
       </c>
       <c r="B24" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E24,F24,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00338#0000</v>
+        <v>obj_0047f#0000</v>
       </c>
       <c r="C24" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B24,OisEngine)</f>
         <v>1</v>
       </c>
       <c r="D24" s="11" t="str">
-        <f>Currency&amp;A24&amp;"x"&amp;A24+6&amp;"F"&amp;QuoteSuffix</f>
+        <f t="shared" si="10"/>
         <v>USD6x12F_Quote</v>
       </c>
       <c r="E24" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,A24&amp;"M","mf")</f>
-        <v>41939</v>
+        <v>41950</v>
       </c>
       <c r="F24" s="56">
         <f>_xll.qlInterestRateIndexMaturity($A$17,E24)</f>
-        <v>42121</v>
+        <v>42131</v>
       </c>
       <c r="G24" s="27">
         <f>_xll.qlQuoteValue(D24,AllTriggers)</f>
-        <v>3.7299999999999998E-3</v>
+        <v>3.7799999999999999E-3</v>
       </c>
       <c r="H24" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B24,_xll.ohTrigger(C24,InterestRatesTrigger))</f>
-        <v>1.4933611316396166E-3</v>
+        <v>1.5839970313506456E-3</v>
       </c>
       <c r="I24" s="16">
-        <f t="shared" si="10"/>
-        <v>2.2366388683603832E-3</v>
+        <f t="shared" si="11"/>
+        <v>2.1960029686493542E-3</v>
       </c>
       <c r="J24" s="1" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="K24" s="15">
         <f>(I24-_xll.ohFilter($I$15:$I$18,$J$15:$J$18))/(P24-_xll.ohFilter($P$15:$P$18,$J$15:$J$18))</f>
-        <v>-3.7088055607638353E-9</v>
+        <v>-6.0667375862611227E-8</v>
       </c>
       <c r="L24" s="15">
         <f>_xll.ohFilter($I$15:$I$18,$J$15:$J$18)-K24*_xll.ohFilter($P$15:$P$18,$J$15:$J$18)</f>
-        <v>2.2386861290299249E-3</v>
+        <v>2.2293093579979278E-3</v>
       </c>
       <c r="M24" s="5"/>
       <c r="N24" s="121">
         <f t="shared" si="2"/>
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O24" s="121">
         <f t="shared" si="3"/>
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="P24" s="121">
         <f t="shared" si="7"/>
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="R24" s="100">
         <f t="shared" si="8"/>
-        <v>78936.333333333328</v>
+        <v>78080.333333333343</v>
       </c>
       <c r="S24" s="100">
         <f t="shared" si="9"/>
-        <v>276</v>
+        <v>274.5</v>
       </c>
       <c r="T24" s="100">
         <v>1</v>
@@ -9878,7 +9876,7 @@
       </c>
       <c r="B25" s="28" t="str">
         <f>_xll.qlMakeDatedOIS(,E25,F25,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0033a#0000</v>
+        <v>obj_00477#0000</v>
       </c>
       <c r="C25" s="8" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B25,OisEngine)</f>
@@ -9890,23 +9888,23 @@
       </c>
       <c r="E25" s="112">
         <f>SettlementDate</f>
-        <v>41754</v>
+        <v>41766</v>
       </c>
       <c r="F25" s="113">
         <f>_xll.qlCalendarAdvance(Calendar,E25,A26,"mf")</f>
-        <v>42121</v>
+        <v>42131</v>
       </c>
       <c r="G25" s="114">
         <f>_xll.qlQuoteValue($D25,AllTriggers)</f>
-        <v>5.483E-3</v>
+        <v>5.4749999999999998E-3</v>
       </c>
       <c r="H25" s="115">
         <f>_xll.qlOvernightIndexedSwapFairRate(B25,_xll.ohTrigger(C25,InterestRatesTrigger))</f>
-        <v>1.2399999999967541E-3</v>
+        <v>1.2899999999996363E-3</v>
       </c>
       <c r="I25" s="116">
         <f t="shared" si="1"/>
-        <v>4.2430000000032459E-3</v>
+        <v>4.1850000000003638E-3</v>
       </c>
       <c r="J25" s="117" t="b">
         <v>0</v>
@@ -9920,33 +9918,33 @@
       </c>
       <c r="O25" s="120">
         <f t="shared" si="3"/>
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="P25" s="120">
         <f t="shared" si="7"/>
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="Q25" s="117"/>
       <c r="R25" s="131">
         <f t="shared" si="8"/>
-        <v>44896.333333333336</v>
+        <v>44408.333333333328</v>
       </c>
       <c r="S25" s="131">
         <f t="shared" si="9"/>
-        <v>183.5</v>
+        <v>182.5</v>
       </c>
       <c r="T25" s="131">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A26" s="238" t="str">
+      <c r="A26" s="232" t="str">
         <f>_xll.qlPeriodEquivalent(A25&amp;"M")</f>
         <v>1Y</v>
       </c>
       <c r="B26" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E26,F26,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0033b#0001</v>
+        <v>obj_0048e#0000</v>
       </c>
       <c r="C26" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B26,OisEngine)</f>
@@ -9958,23 +9956,23 @@
       </c>
       <c r="E26" s="105">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlLastFixingQuoteReferenceDate(D26),_xll.qlInterestRateIndexFixingDays(A27)&amp;"D","f",,LastFixingsTrigger)</f>
-        <v>41754</v>
+        <v>41765</v>
       </c>
       <c r="F26" s="106">
         <f>_xll.qlInterestRateIndexMaturity(A27,E26)</f>
-        <v>42121</v>
+        <v>42130</v>
       </c>
       <c r="G26" s="107">
         <f>_xll.qlQuoteValue(D26,AllTriggers)</f>
-        <v>5.483E-3</v>
+        <v>5.4749999999999998E-3</v>
       </c>
       <c r="H26" s="108">
         <f>_xll.qlOvernightIndexedSwapFairRate(B26,_xll.ohTrigger(C26,InterestRatesTrigger))</f>
-        <v>1.2399999999967541E-3</v>
+        <v>1.2875088968702711E-3</v>
       </c>
       <c r="I26" s="109">
         <f t="shared" si="1"/>
-        <v>4.2430000000032459E-3</v>
+        <v>4.1874911031297285E-3</v>
       </c>
       <c r="J26" s="117" t="b">
         <f>NOT(ISERROR(I26))</f>
@@ -9991,37 +9989,37 @@
       <c r="M26" s="118"/>
       <c r="N26" s="120">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O26" s="120">
         <f t="shared" si="3"/>
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="P26" s="120">
         <f t="shared" si="7"/>
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="Q26" s="117"/>
       <c r="R26" s="131">
         <f t="shared" si="8"/>
-        <v>44896.333333333336</v>
+        <v>44044.333333333328</v>
       </c>
       <c r="S26" s="131">
         <f t="shared" si="9"/>
-        <v>183.5</v>
+        <v>181.5</v>
       </c>
       <c r="T26" s="131">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A27" s="238" t="str">
+      <c r="A27" s="232" t="str">
         <f>PROPER(Currency)&amp;IborType&amp;A26</f>
         <v>UsdLibor1Y</v>
       </c>
       <c r="B27" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E27,F27,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0033c#0000</v>
+        <v>obj_0046d#0000</v>
       </c>
       <c r="C27" s="12" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B27,OisEngine)</f>
@@ -10033,11 +10031,11 @@
       </c>
       <c r="E27" s="55">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,"12M","mf")</f>
-        <v>42121</v>
+        <v>42131</v>
       </c>
       <c r="F27" s="56">
         <f>_xll.qlInterestRateIndexMaturity(A27,E27)</f>
-        <v>42487</v>
+        <v>42499</v>
       </c>
       <c r="G27" s="27" t="e">
         <f>_xll.qlQuoteValue(D27,AllTriggers)</f>
@@ -10045,7 +10043,7 @@
       </c>
       <c r="H27" s="15">
         <f>_xll.qlOvernightIndexedSwapFairRate(B27,_xll.ohTrigger(C27,InterestRatesTrigger))</f>
-        <v>6.3740210273735328E-3</v>
+        <v>6.2655189115717888E-3</v>
       </c>
       <c r="I27" s="16" t="e">
         <f t="shared" si="1"/>
@@ -10066,7 +10064,7 @@
       <c r="M27" s="5"/>
       <c r="N27" s="121">
         <f t="shared" si="2"/>
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="O27" s="121">
         <f t="shared" si="3"/>
@@ -10074,15 +10072,15 @@
       </c>
       <c r="P27" s="121">
         <f t="shared" si="7"/>
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="R27" s="100">
         <f t="shared" si="8"/>
-        <v>313663</v>
+        <v>312686.33333333337</v>
       </c>
       <c r="S27" s="100">
         <f t="shared" si="9"/>
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="T27" s="100">
         <v>1</v>
@@ -10153,11 +10151,11 @@
       </c>
       <c r="V30" s="126">
         <f>Z9</f>
-        <v>2.4255205846153995E-8</v>
+        <v>3.1587917154378896E-8</v>
       </c>
       <c r="W30" s="13">
         <f>Z18</f>
-        <v>2.0400485387877149E-8</v>
+        <v>1.8183142703755349E-8</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.2">
@@ -10166,34 +10164,34 @@
       </c>
       <c r="G31" s="37">
         <f>_xll.ohFilter(I2:I3,J2:J3)</f>
-        <v>6.1201416720313743E-4</v>
+        <v>6.0499999994202442E-4</v>
       </c>
       <c r="H31" s="38">
         <f>_xll.ohFilter(I6:I9,J6:J9)</f>
-        <v>1.3674999999999462E-3</v>
+        <v>1.2985000005329545E-3</v>
       </c>
       <c r="I31" s="38">
         <f>_xll.ohFilter(I15:I18,J15:J18)</f>
-        <v>2.2380000000011835E-3</v>
+        <v>2.2182678955909325E-3</v>
       </c>
       <c r="J31" s="39">
         <f>_xll.ohFilter(I25:I26,J25:J26)</f>
-        <v>4.2430000000032459E-3</v>
+        <v>4.1874911031297285E-3</v>
       </c>
       <c r="M31" s="67" t="s">
         <v>46</v>
       </c>
       <c r="N31" s="66">
         <f>K4</f>
-        <v>-7.163187341494072E-8</v>
+        <v>-5.3786613586453301E-7</v>
       </c>
       <c r="O31" s="66">
         <f>K9</f>
-        <v>-3.7175264097954424E-7</v>
+        <v>-8.0180558696483716E-7</v>
       </c>
       <c r="P31" s="66">
         <f>AVERAGE(K19:K21)</f>
-        <v>-2.6339997809853552E-7</v>
+        <v>-5.814751652831254E-7</v>
       </c>
       <c r="Q31" s="66" t="e">
         <f>K26</f>
@@ -10204,11 +10202,11 @@
       </c>
       <c r="V31" s="72">
         <f>Z10</f>
-        <v>-3.8647513651200672E-6</v>
+        <v>-5.4804670963328801E-6</v>
       </c>
       <c r="W31" s="16">
         <f>Z19</f>
-        <v>-5.3331298056535285E-6</v>
+        <v>-5.4771463108833191E-6</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.2">
@@ -10217,34 +10215,34 @@
       </c>
       <c r="G32" s="37">
         <f>IF(G31&lt;H31,G31,H31)</f>
-        <v>6.1201416720313743E-4</v>
+        <v>6.0499999994202442E-4</v>
       </c>
       <c r="H32" s="38">
         <f>H31</f>
-        <v>1.3674999999999462E-3</v>
+        <v>1.2985000005329545E-3</v>
       </c>
       <c r="I32" s="38">
         <f>IF(I31&lt;H31,H31,I31)</f>
-        <v>2.2380000000011835E-3</v>
+        <v>2.2182678955909325E-3</v>
       </c>
       <c r="J32" s="39">
         <f>IF(J31&lt;I31,I31,J31)</f>
-        <v>4.2430000000032459E-3</v>
+        <v>4.1874911031297285E-3</v>
       </c>
       <c r="M32" s="67" t="s">
         <v>45</v>
       </c>
       <c r="N32" s="66">
         <f>L4</f>
-        <v>6.143063871524155E-4</v>
+        <v>6.2274958242555399E-4</v>
       </c>
       <c r="O32" s="66">
         <f>L9</f>
-        <v>1.4013294903290848E-3</v>
+        <v>1.3722661145337196E-3</v>
       </c>
       <c r="P32" s="66">
         <f>L18</f>
-        <v>2.2867289959494124E-3</v>
+        <v>2.3240963756724613E-3</v>
       </c>
       <c r="Q32" s="66" t="e">
         <f>L26</f>
@@ -10255,11 +10253,11 @@
       </c>
       <c r="V32" s="72">
         <f>Z11</f>
-        <v>1.4763937339089097E-3</v>
+        <v>1.461481443366048E-3</v>
       </c>
       <c r="W32" s="16">
         <f>Z20</f>
-        <v>2.4985789695574408E-3</v>
+        <v>2.514812898536653E-3</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
@@ -10317,7 +10315,7 @@
     <row r="34" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B34" s="132" t="str">
         <f>_xll.qlMakeDatedOIS(,E34,F34,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00331#0000</v>
+        <v>obj_0047d#0000</v>
       </c>
       <c r="C34" s="7" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B34,OisEngine)</f>
@@ -10327,69 +10325,69 @@
         <v>14</v>
       </c>
       <c r="E34" s="53">
-        <f t="shared" ref="E34:E49" si="12">SettlementDate</f>
-        <v>41754</v>
+        <f t="shared" ref="E34:E49" si="13">SettlementDate</f>
+        <v>41766</v>
       </c>
       <c r="F34" s="22">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D34,"Following")</f>
-        <v>41757</v>
+        <v>41767</v>
       </c>
       <c r="G34" s="32">
-        <f t="shared" ref="G34:J38" si="13">$L34+IF(G$30,G$32,N34)</f>
-        <v>1.4640914902387782E-3</v>
+        <f t="shared" ref="G34:J38" si="14">$L34+IF(G$30,G$32,N34)</f>
+        <v>1.5222117163012955E-3</v>
       </c>
       <c r="H34" s="32">
-        <f t="shared" si="13"/>
-        <v>2.3206693711853759E-3</v>
+        <f t="shared" si="14"/>
+        <v>2.3587517391352054E-3</v>
       </c>
       <c r="I34" s="32">
-        <f t="shared" si="13"/>
-        <v>3.340640475011732E-3</v>
+        <f t="shared" si="14"/>
+        <v>3.4120803864403854E-3</v>
       </c>
       <c r="J34" s="32">
-        <f t="shared" si="13"/>
-        <v>5.0929999987098535E-3</v>
+        <f t="shared" si="14"/>
+        <v>5.0874911031413344E-3</v>
       </c>
       <c r="K34" s="133">
         <f>F34-$E$6</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L34" s="2">
         <f>L35</f>
-        <v>8.4999999870660758E-4</v>
+        <v>9.0000000001160593E-4</v>
       </c>
       <c r="N34" s="71">
         <f>N$31*$K34+N$32</f>
-        <v>6.1409149153217064E-4</v>
+        <v>6.2221171628968946E-4</v>
       </c>
       <c r="O34" s="72">
-        <f t="shared" ref="O34:P40" si="14">IF(O$30,V34,O$31*$K34+O$32)</f>
-        <v>1.4706693724787681E-3</v>
+        <f t="shared" ref="O34:P40" si="15">IF(O$30,V34,O$31*$K34+O$32)</f>
+        <v>1.4587517391235997E-3</v>
       </c>
       <c r="P34" s="72">
-        <f t="shared" si="14"/>
-        <v>2.4906404763051244E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.5120803864287795E-3</v>
       </c>
       <c r="Q34" s="16" t="e">
-        <f t="shared" ref="Q34:Q49" si="15">Q$31*$K34+Q$32</f>
+        <f t="shared" ref="Q34:Q49" si="16">Q$31*$K34+Q$32</f>
         <v>#NUM!</v>
       </c>
       <c r="U34" s="21" t="s">
         <v>14</v>
       </c>
       <c r="V34" s="72">
-        <f t="shared" ref="V34:W40" si="16">$K34*$K34/3*V$30+$K34/2*V$31+V$32</f>
-        <v>1.4706693724787681E-3</v>
+        <f t="shared" ref="V34:W40" si="17">$K34*$K34/3*V$30+$K34/2*V$31+V$32</f>
+        <v>1.4587517391235997E-3</v>
       </c>
       <c r="W34" s="16">
-        <f t="shared" si="16"/>
-        <v>2.4906404763051244E-3</v>
+        <f t="shared" si="17"/>
+        <v>2.5120803864287795E-3</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B35" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E35,F35,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00280#0000</v>
+        <v>obj_00483#0000</v>
       </c>
       <c r="C35" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B35,OisEngine)</f>
@@ -10399,69 +10397,69 @@
         <v>4</v>
       </c>
       <c r="E35" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F35" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D35,"Following")</f>
-        <v>41761</v>
+        <v>41773</v>
       </c>
       <c r="G35" s="32">
-        <f t="shared" si="13"/>
-        <v>1.4638049627451184E-3</v>
+        <f t="shared" si="14"/>
+        <v>1.5189845194861083E-3</v>
       </c>
       <c r="H35" s="32">
-        <f t="shared" si="13"/>
-        <v>2.3132632711997509E-3</v>
+        <f t="shared" si="14"/>
+        <v>2.3428157445206771E-3</v>
       </c>
       <c r="I35" s="32">
-        <f t="shared" si="13"/>
-        <v>3.330246221872263E-3</v>
+        <f t="shared" si="14"/>
+        <v>3.3959398777909954E-3</v>
       </c>
       <c r="J35" s="32">
-        <f t="shared" si="13"/>
-        <v>5.0929999987098535E-3</v>
+        <f t="shared" si="14"/>
+        <v>5.0874911031413344E-3</v>
       </c>
       <c r="K35" s="134">
-        <f t="shared" ref="K35:K49" si="17">F35-$E$6</f>
+        <f t="shared" ref="K35:K49" si="18">F35-$E$6</f>
         <v>7</v>
       </c>
       <c r="L35" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B35,_xll.ohTrigger(C35,InterestRatesTrigger))</f>
-        <v>8.4999999870660758E-4</v>
+        <v>9.0000000001160593E-4</v>
       </c>
       <c r="N35" s="71">
         <f>N$31*$K35+N$32</f>
-        <v>6.1380496403851093E-4</v>
+        <v>6.1898451947450231E-4</v>
       </c>
       <c r="O35" s="72">
-        <f t="shared" si="14"/>
-        <v>1.4632632724931433E-3</v>
+        <f t="shared" si="15"/>
+        <v>1.4428157445090712E-3</v>
       </c>
       <c r="P35" s="72">
-        <f t="shared" si="14"/>
-        <v>2.4802462231656554E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.4959398777793895E-3</v>
       </c>
       <c r="Q35" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U35" s="23" t="s">
         <v>4</v>
       </c>
       <c r="V35" s="72">
-        <f t="shared" si="16"/>
-        <v>1.4632632724931433E-3</v>
+        <f t="shared" si="17"/>
+        <v>1.4428157445090712E-3</v>
       </c>
       <c r="W35" s="16">
-        <f t="shared" si="16"/>
-        <v>2.4802462231656554E-3</v>
+        <f t="shared" si="17"/>
+        <v>2.4959398777793895E-3</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B36" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E36,F36,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00275#0000</v>
+        <v>obj_00479#0000</v>
       </c>
       <c r="C36" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B36,OisEngine)</f>
@@ -10471,69 +10469,69 @@
         <v>5</v>
       </c>
       <c r="E36" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F36" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D36,"Following")</f>
-        <v>41768</v>
+        <v>41780</v>
       </c>
       <c r="G36" s="32">
-        <f t="shared" si="13"/>
-        <v>1.5033035367629133E-3</v>
+        <f t="shared" si="14"/>
+        <v>1.515219457614193E-3</v>
       </c>
       <c r="H36" s="32">
-        <f t="shared" si="13"/>
-        <v>2.3409251436399916E-3</v>
+        <f t="shared" si="14"/>
+        <v>2.3251819187032133E-3</v>
       </c>
       <c r="I36" s="32">
-        <f t="shared" si="13"/>
-        <v>3.352579888468181E-3</v>
+        <f t="shared" si="14"/>
+        <v>3.377660840774524E-3</v>
       </c>
       <c r="J36" s="32">
-        <f t="shared" si="13"/>
-        <v>5.1329999958415525E-3</v>
+        <f t="shared" si="14"/>
+        <v>5.0874911042204712E-3</v>
       </c>
       <c r="K36" s="134">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>14</v>
       </c>
       <c r="L36" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B36,_xll.ohTrigger(C36,InterestRatesTrigger))</f>
-        <v>8.8999999583830693E-4</v>
+        <v>9.0000000109074249E-4</v>
       </c>
       <c r="N36" s="71">
         <f>N$31*$K36+N$32</f>
-        <v>6.1330354092460637E-4</v>
+        <v>6.1521945652345052E-4</v>
       </c>
       <c r="O36" s="72">
-        <f t="shared" si="14"/>
-        <v>1.4509251478016846E-3</v>
+        <f t="shared" si="15"/>
+        <v>1.4251819176124706E-3</v>
       </c>
       <c r="P36" s="72">
-        <f t="shared" si="14"/>
-        <v>2.462579892629874E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.4776608396837817E-3</v>
       </c>
       <c r="Q36" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U36" s="23" t="s">
         <v>5</v>
       </c>
       <c r="V36" s="72">
-        <f t="shared" si="16"/>
-        <v>1.4509251478016846E-3</v>
+        <f t="shared" si="17"/>
+        <v>1.4251819176124706E-3</v>
       </c>
       <c r="W36" s="16">
-        <f t="shared" si="16"/>
-        <v>2.462579892629874E-3</v>
+        <f t="shared" si="17"/>
+        <v>2.4776608396837817E-3</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B37" s="30" t="str">
         <f>_xll.qlMakeDatedOIS(,E37,F37,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00284#0000</v>
+        <v>obj_0046e#0000</v>
       </c>
       <c r="C37" s="10" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B37,OisEngine)</f>
@@ -10543,69 +10541,69 @@
         <v>8</v>
       </c>
       <c r="E37" s="54">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F37" s="26">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D37,"Following")</f>
-        <v>41775</v>
+        <v>41787</v>
       </c>
       <c r="G37" s="35">
-        <f t="shared" si="13"/>
-        <v>1.5128021123447842E-3</v>
+        <f t="shared" si="14"/>
+        <v>1.5114543904398529E-3</v>
       </c>
       <c r="H37" s="35">
-        <f t="shared" si="13"/>
-        <v>2.339379354368616E-3</v>
+        <f t="shared" si="14"/>
+        <v>2.3085799595437008E-3</v>
       </c>
       <c r="I37" s="35">
-        <f t="shared" si="13"/>
-        <v>3.3455799724841791E-3</v>
+        <f t="shared" si="14"/>
+        <v>3.3599757811172844E-3</v>
       </c>
       <c r="J37" s="35">
-        <f t="shared" si="13"/>
-        <v>5.142999994537328E-3</v>
+        <f t="shared" si="14"/>
+        <v>5.0874910999971828E-3</v>
       </c>
       <c r="K37" s="135">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="L37" s="4">
         <f>_xll.qlOvernightIndexedSwapFairRate(B37,_xll.ohTrigger(C37,InterestRatesTrigger))</f>
-        <v>8.9999999453408254E-4</v>
+        <v>8.9999999686745421E-4</v>
       </c>
       <c r="N37" s="101">
         <f>N$31*$K37+N$32</f>
-        <v>6.128021178107017E-4</v>
+        <v>6.1145439357239884E-4</v>
       </c>
       <c r="O37" s="102">
-        <f t="shared" si="14"/>
-        <v>1.4393793598345337E-3</v>
+        <f t="shared" si="15"/>
+        <v>1.4085799626762465E-3</v>
       </c>
       <c r="P37" s="102">
-        <f t="shared" si="14"/>
-        <v>2.4455799779500966E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.4599757842498301E-3</v>
       </c>
       <c r="Q37" s="14" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U37" s="31" t="s">
         <v>8</v>
       </c>
       <c r="V37" s="102">
-        <f t="shared" si="16"/>
-        <v>1.4393793598345337E-3</v>
+        <f t="shared" si="17"/>
+        <v>1.4085799626762465E-3</v>
       </c>
       <c r="W37" s="14">
-        <f t="shared" si="16"/>
-        <v>2.4455799779500966E-3</v>
+        <f t="shared" si="17"/>
+        <v>2.4599757842498301E-3</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B38" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E38,F38,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0027b#0000</v>
+        <v>obj_0048b#0000</v>
       </c>
       <c r="C38" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B38,OisEngine)</f>
@@ -10615,69 +10613,69 @@
         <v>9</v>
       </c>
       <c r="E38" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F38" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D38,"mf",TRUE)</f>
-        <v>41786</v>
+        <v>41799</v>
       </c>
       <c r="G38" s="34">
-        <f t="shared" si="13"/>
-        <v>1.5229999999999998E-3</v>
+        <f t="shared" si="14"/>
+        <v>1.505E-3</v>
       </c>
       <c r="H38" s="34">
-        <f t="shared" si="13"/>
-        <v>2.3338226551260048E-3</v>
+        <f t="shared" si="14"/>
+        <v>2.2825201502615707E-3</v>
       </c>
       <c r="I38" s="34">
-        <f t="shared" si="13"/>
-        <v>3.3311980911429088E-3</v>
+        <f t="shared" si="14"/>
+        <v>3.3310404652665171E-3</v>
       </c>
       <c r="J38" s="34">
-        <f t="shared" si="13"/>
-        <v>5.1539858328001082E-3</v>
+        <f t="shared" si="14"/>
+        <v>5.0874911031877044E-3</v>
       </c>
       <c r="K38" s="133">
-        <f t="shared" si="17"/>
-        <v>32</v>
+        <f t="shared" si="18"/>
+        <v>33</v>
       </c>
       <c r="L38" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B38,_xll.ohTrigger(C38,InterestRatesTrigger))</f>
-        <v>9.109858327968624E-4</v>
+        <v>9.0000000005797563E-4</v>
       </c>
       <c r="N38" s="71">
         <f>N$31*$K38+N$32</f>
-        <v>6.1201416720313743E-4</v>
+        <v>6.0499999994202442E-4</v>
       </c>
       <c r="O38" s="72">
-        <f t="shared" si="14"/>
-        <v>1.4228368223291425E-3</v>
+        <f t="shared" si="15"/>
+        <v>1.3825201502035949E-3</v>
       </c>
       <c r="P38" s="72">
-        <f t="shared" si="14"/>
-        <v>2.4202122583460465E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.4310404652085416E-3</v>
       </c>
       <c r="Q38" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U38" s="23" t="s">
         <v>9</v>
       </c>
       <c r="V38" s="72">
-        <f t="shared" si="16"/>
-        <v>1.4228368223291425E-3</v>
+        <f t="shared" si="17"/>
+        <v>1.3825201502035949E-3</v>
       </c>
       <c r="W38" s="16">
-        <f t="shared" si="16"/>
-        <v>2.4202122583460465E-3</v>
+        <f t="shared" si="17"/>
+        <v>2.4310404652085416E-3</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B39" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E39,F39,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00276#0000</v>
+        <v>obj_0047b#0000</v>
       </c>
       <c r="C39" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B39,OisEngine)</f>
@@ -10687,63 +10685,63 @@
         <v>10</v>
       </c>
       <c r="E39" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F39" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D39,"mf",TRUE)</f>
-        <v>41815</v>
+        <v>41827</v>
       </c>
       <c r="G39" s="49"/>
       <c r="H39" s="32">
-        <f t="shared" ref="H39:J40" si="18">$L39+IF(H$30,H$32,O39)</f>
-        <v>2.3086033575903308E-3</v>
+        <f t="shared" ref="H39:J40" si="19">$L39+IF(H$30,H$32,O39)</f>
+        <v>2.2535067435047801E-3</v>
       </c>
       <c r="I39" s="32">
+        <f t="shared" si="19"/>
+        <v>3.2903130940546733E-3</v>
+      </c>
+      <c r="J39" s="32">
+        <f t="shared" si="19"/>
+        <v>5.1074911031294655E-3</v>
+      </c>
+      <c r="K39" s="134">
         <f t="shared" si="18"/>
-        <v>3.2812219125275088E-3</v>
-      </c>
-      <c r="J39" s="32">
-        <f t="shared" si="18"/>
-        <v>5.1630000000029829E-3</v>
-      </c>
-      <c r="K39" s="134">
-        <f t="shared" si="17"/>
         <v>61</v>
       </c>
       <c r="L39" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B39,_xll.ohTrigger(C39,InterestRatesTrigger))</f>
-        <v>9.1999999999973689E-4</v>
+        <v>9.19999999999737E-4</v>
       </c>
       <c r="N39" s="49"/>
       <c r="O39" s="72">
-        <f t="shared" si="14"/>
-        <v>1.388603357590594E-3</v>
+        <f t="shared" si="15"/>
+        <v>1.3335067435050431E-3</v>
       </c>
       <c r="P39" s="72">
-        <f t="shared" si="14"/>
-        <v>2.3612219125277718E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.3703130940549363E-3</v>
       </c>
       <c r="Q39" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U39" s="23" t="s">
         <v>10</v>
       </c>
       <c r="V39" s="72">
-        <f t="shared" si="16"/>
-        <v>1.388603357590594E-3</v>
+        <f t="shared" si="17"/>
+        <v>1.3335067435050431E-3</v>
       </c>
       <c r="W39" s="16">
-        <f t="shared" si="16"/>
-        <v>2.3612219125277718E-3</v>
+        <f t="shared" si="17"/>
+        <v>2.3703130940549363E-3</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B40" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E40,F40,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0027d#0000</v>
+        <v>obj_00478#0000</v>
       </c>
       <c r="C40" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B40,OisEngine)</f>
@@ -10753,63 +10751,63 @@
         <v>3</v>
       </c>
       <c r="E40" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F40" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D40,"mf",TRUE)</f>
-        <v>41845</v>
+        <v>41858</v>
       </c>
       <c r="G40" s="47"/>
       <c r="H40" s="32">
+        <f t="shared" si="19"/>
+        <v>2.2285000000000022E-3</v>
+      </c>
+      <c r="I40" s="32">
+        <f t="shared" si="19"/>
+        <v>3.2441648743179274E-3</v>
+      </c>
+      <c r="J40" s="32">
+        <f t="shared" si="19"/>
+        <v>5.117491102596774E-3</v>
+      </c>
+      <c r="K40" s="134">
         <f t="shared" si="18"/>
-        <v>2.2875000000000009E-3</v>
-      </c>
-      <c r="I40" s="32">
-        <f t="shared" si="18"/>
-        <v>3.2322337032325956E-3</v>
-      </c>
-      <c r="J40" s="32">
-        <f t="shared" si="18"/>
-        <v>5.1630000000032995E-3</v>
-      </c>
-      <c r="K40" s="134">
-        <f t="shared" si="17"/>
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L40" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B40,_xll.ohTrigger(C40,InterestRatesTrigger))</f>
-        <v>9.200000000000538E-4</v>
+        <v>9.2999999946704562E-4</v>
       </c>
       <c r="N40" s="47"/>
       <c r="O40" s="72">
-        <f t="shared" si="14"/>
-        <v>1.3674999999999471E-3</v>
+        <f t="shared" si="15"/>
+        <v>1.2985000005329567E-3</v>
       </c>
       <c r="P40" s="72">
-        <f t="shared" si="14"/>
-        <v>2.312233703232542E-3</v>
+        <f t="shared" si="15"/>
+        <v>2.3141648748508819E-3</v>
       </c>
       <c r="Q40" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U40" s="23" t="s">
         <v>3</v>
       </c>
       <c r="V40" s="72">
-        <f t="shared" si="16"/>
-        <v>1.3674999999999471E-3</v>
+        <f t="shared" si="17"/>
+        <v>1.2985000005329567E-3</v>
       </c>
       <c r="W40" s="16">
-        <f t="shared" si="16"/>
-        <v>2.312233703232542E-3</v>
+        <f t="shared" si="17"/>
+        <v>2.3141648748508819E-3</v>
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B41" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E41,F41,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00277#0000</v>
+        <v>obj_00484#0000</v>
       </c>
       <c r="C41" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B41,OisEngine)</f>
@@ -10819,39 +10817,39 @@
         <v>12</v>
       </c>
       <c r="E41" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F41" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D41,"mf",TRUE)</f>
-        <v>41877</v>
+        <v>41890</v>
       </c>
       <c r="G41" s="36"/>
       <c r="H41" s="48"/>
       <c r="I41" s="32">
-        <f t="shared" ref="I41:J43" si="19">$L41+IF(I$30,I$32,P41)</f>
-        <v>3.2141301064413756E-3</v>
+        <f t="shared" ref="I41:J43" si="20">$L41+IF(I$30,I$32,P41)</f>
+        <v>3.2184244950372947E-3</v>
       </c>
       <c r="J41" s="32">
-        <f t="shared" si="19"/>
-        <v>5.1836589721238084E-3</v>
+        <f t="shared" si="20"/>
+        <v>5.1374911035008217E-3</v>
       </c>
       <c r="K41" s="134">
-        <f t="shared" si="17"/>
-        <v>123</v>
+        <f t="shared" si="18"/>
+        <v>124</v>
       </c>
       <c r="L41" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B41,_xll.ohTrigger(C41,InterestRatesTrigger))</f>
-        <v>9.4065897212056247E-4</v>
+        <v>9.5000000037109324E-4</v>
       </c>
       <c r="N41" s="36"/>
       <c r="O41" s="48"/>
       <c r="P41" s="72">
         <f>IF(P$30,W41,P$31*$K41+P$32)</f>
-        <v>2.2734711343208132E-3</v>
+        <v>2.2684244946662015E-3</v>
       </c>
       <c r="Q41" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U41" s="23" t="s">
@@ -10860,13 +10858,13 @@
       <c r="V41" s="72"/>
       <c r="W41" s="16">
         <f>$K41*$K41/3*W$30+$K41/2*W$31+W$32</f>
-        <v>2.2734711343208132E-3</v>
+        <v>2.2684244946662015E-3</v>
       </c>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B42" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E42,F42,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0027f#0000</v>
+        <v>obj_0047c#0000</v>
       </c>
       <c r="C42" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B42,OisEngine)</f>
@@ -10876,39 +10874,39 @@
         <v>13</v>
       </c>
       <c r="E42" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F42" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D42,"mf",TRUE)</f>
-        <v>41907</v>
+        <v>41919</v>
       </c>
       <c r="G42" s="36"/>
       <c r="H42" s="46"/>
       <c r="I42" s="32">
-        <f t="shared" si="19"/>
-        <v>3.2097795269059441E-3</v>
+        <f t="shared" si="20"/>
+        <v>3.2076942677200346E-3</v>
       </c>
       <c r="J42" s="32">
-        <f t="shared" si="19"/>
-        <v>5.2030000000026387E-3</v>
+        <f t="shared" si="20"/>
+        <v>5.1574911025782811E-3</v>
       </c>
       <c r="K42" s="134">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>153</v>
       </c>
       <c r="L42" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B42,_xll.ohTrigger(C42,InterestRatesTrigger))</f>
-        <v>9.5999999999939287E-4</v>
+        <v>9.6999999944855249E-4</v>
       </c>
       <c r="N42" s="36"/>
       <c r="O42" s="46"/>
       <c r="P42" s="72">
         <f>IF(P$30,W42,P$31*$K42+P$32)</f>
-        <v>2.2497795269065513E-3</v>
+        <v>2.237694268271482E-3</v>
       </c>
       <c r="Q42" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U42" s="23" t="s">
@@ -10917,13 +10915,13 @@
       <c r="V42" s="72"/>
       <c r="W42" s="16">
         <f>$K42*$K42/3*W$30+$K42/2*W$31+W$32</f>
-        <v>2.2497795269065513E-3</v>
+        <v>2.237694268271482E-3</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B43" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E43,F43,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0027e#0000</v>
+        <v>obj_0047a#0000</v>
       </c>
       <c r="C43" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B43,OisEngine)</f>
@@ -10933,39 +10931,39 @@
         <v>15</v>
       </c>
       <c r="E43" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F43" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D43,"mf",TRUE)</f>
-        <v>41939</v>
+        <v>41950</v>
       </c>
       <c r="G43" s="36"/>
       <c r="H43" s="46"/>
       <c r="I43" s="32">
-        <f t="shared" si="19"/>
-        <v>3.2280000000000043E-3</v>
+        <f t="shared" si="20"/>
+        <v>3.2161182643953038E-3</v>
       </c>
       <c r="J43" s="32">
-        <f t="shared" si="19"/>
-        <v>5.2330000000020624E-3</v>
+        <f t="shared" si="20"/>
+        <v>5.1874911031301978E-3</v>
       </c>
       <c r="K43" s="134">
-        <f t="shared" si="17"/>
-        <v>185</v>
+        <f t="shared" si="18"/>
+        <v>184</v>
       </c>
       <c r="L43" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B43,_xll.ohTrigger(C43,InterestRatesTrigger))</f>
-        <v>9.8999999999881626E-4</v>
+        <v>1.0000000000004693E-3</v>
       </c>
       <c r="N43" s="36"/>
       <c r="O43" s="46"/>
       <c r="P43" s="72">
         <f>IF(P$30,W43,P$31*$K43+P$32)</f>
-        <v>2.2380000000011878E-3</v>
+        <v>2.2161182643948346E-3</v>
       </c>
       <c r="Q43" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
       <c r="U43" s="129" t="s">
@@ -10974,13 +10972,13 @@
       <c r="V43" s="102"/>
       <c r="W43" s="14">
         <f>$K43*$K43/3*W$30+$K43/2*W$31+W$32</f>
-        <v>2.2380000000011878E-3</v>
+        <v>2.2161182643948346E-3</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B44" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E44,F44,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00283#0000</v>
+        <v>obj_0046f#0000</v>
       </c>
       <c r="C44" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B44,OisEngine)</f>
@@ -10990,40 +10988,40 @@
         <v>18</v>
       </c>
       <c r="E44" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F44" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D44,"mf",TRUE)</f>
-        <v>41968</v>
+        <v>41981</v>
       </c>
       <c r="G44" s="36"/>
       <c r="H44" s="33"/>
       <c r="I44" s="48"/>
       <c r="J44" s="32">
-        <f t="shared" ref="J44:J49" si="20">$L44+IF(J$30,J$32,Q44)</f>
-        <v>5.2630000000020091E-3</v>
+        <f t="shared" ref="J44:J49" si="21">$L44+IF(J$30,J$32,Q44)</f>
+        <v>5.2174911031296917E-3</v>
       </c>
       <c r="K44" s="134">
-        <f t="shared" si="17"/>
-        <v>214</v>
+        <f t="shared" si="18"/>
+        <v>215</v>
       </c>
       <c r="L44" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B44,_xll.ohTrigger(C44,InterestRatesTrigger))</f>
-        <v>1.0199999999987634E-3</v>
+        <v>1.0299999999999628E-3</v>
       </c>
       <c r="N44" s="36"/>
       <c r="O44" s="33"/>
       <c r="P44" s="48"/>
       <c r="Q44" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B45" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E45,F45,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00281#0000</v>
+        <v>obj_00485#0000</v>
       </c>
       <c r="C45" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B45,OisEngine)</f>
@@ -11033,40 +11031,40 @@
         <v>19</v>
       </c>
       <c r="E45" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F45" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D45,"mf",TRUE)</f>
-        <v>42002</v>
+        <v>42011</v>
       </c>
       <c r="G45" s="36"/>
       <c r="H45" s="33"/>
       <c r="I45" s="46"/>
       <c r="J45" s="32">
-        <f t="shared" si="20"/>
-        <v>5.2830000000010984E-3</v>
+        <f t="shared" si="21"/>
+        <v>5.2474911031296576E-3</v>
       </c>
       <c r="K45" s="134">
-        <f t="shared" si="17"/>
-        <v>248</v>
+        <f t="shared" si="18"/>
+        <v>245</v>
       </c>
       <c r="L45" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B45,_xll.ohTrigger(C45,InterestRatesTrigger))</f>
-        <v>1.0399999999978528E-3</v>
+        <v>1.0599999999999295E-3</v>
       </c>
       <c r="N45" s="36"/>
       <c r="O45" s="33"/>
       <c r="P45" s="46"/>
       <c r="Q45" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B46" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E46,F46,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0027a#0000</v>
+        <v>obj_00481#0000</v>
       </c>
       <c r="C46" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B46,OisEngine)</f>
@@ -11076,40 +11074,40 @@
         <v>20</v>
       </c>
       <c r="E46" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F46" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D46,"mf",TRUE)</f>
-        <v>42030</v>
+        <v>42044</v>
       </c>
       <c r="G46" s="36"/>
       <c r="H46" s="33"/>
       <c r="I46" s="46"/>
       <c r="J46" s="32">
-        <f t="shared" si="20"/>
-        <v>5.323000000001285E-3</v>
+        <f t="shared" si="21"/>
+        <v>5.2874911031297461E-3</v>
       </c>
       <c r="K46" s="134">
-        <f t="shared" si="17"/>
-        <v>276</v>
+        <f t="shared" si="18"/>
+        <v>278</v>
       </c>
       <c r="L46" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B46,_xll.ohTrigger(C46,InterestRatesTrigger))</f>
-        <v>1.0799999999980389E-3</v>
+        <v>1.1000000000000176E-3</v>
       </c>
       <c r="N46" s="36"/>
       <c r="O46" s="33"/>
       <c r="P46" s="46"/>
       <c r="Q46" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B47" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E47,F47,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00285#0000</v>
+        <v>obj_00476#0000</v>
       </c>
       <c r="C47" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B47,OisEngine)</f>
@@ -11119,40 +11117,40 @@
         <v>21</v>
       </c>
       <c r="E47" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F47" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D47,"mf",TRUE)</f>
-        <v>42060</v>
+        <v>42072</v>
       </c>
       <c r="G47" s="36"/>
       <c r="H47" s="33"/>
       <c r="I47" s="46"/>
       <c r="J47" s="32">
-        <f t="shared" si="20"/>
-        <v>5.3730000000013229E-3</v>
+        <f t="shared" si="21"/>
+        <v>5.3374911031298169E-3</v>
       </c>
       <c r="K47" s="134">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>306</v>
       </c>
       <c r="L47" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B47,_xll.ohTrigger(C47,InterestRatesTrigger))</f>
-        <v>1.1299999999980772E-3</v>
+        <v>1.1500000000000889E-3</v>
       </c>
       <c r="N47" s="36"/>
       <c r="O47" s="33"/>
       <c r="P47" s="46"/>
       <c r="Q47" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B48" s="29" t="str">
         <f>_xll.qlMakeDatedOIS(,E48,F48,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_0027c#0000</v>
+        <v>obj_00471#0000</v>
       </c>
       <c r="C48" s="5" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B48,OisEngine)</f>
@@ -11162,40 +11160,40 @@
         <v>22</v>
       </c>
       <c r="E48" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F48" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D48,"mf",TRUE)</f>
-        <v>42088</v>
+        <v>42101</v>
       </c>
       <c r="G48" s="36"/>
       <c r="H48" s="33"/>
       <c r="I48" s="46"/>
       <c r="J48" s="32">
-        <f t="shared" si="20"/>
-        <v>5.4130000000011703E-3</v>
+        <f t="shared" si="21"/>
+        <v>5.397491103129602E-3</v>
       </c>
       <c r="K48" s="134">
-        <f t="shared" si="17"/>
-        <v>334</v>
+        <f t="shared" si="18"/>
+        <v>335</v>
       </c>
       <c r="L48" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B48,_xll.ohTrigger(C48,InterestRatesTrigger))</f>
-        <v>1.1699999999979242E-3</v>
+        <v>1.2099999999998737E-3</v>
       </c>
       <c r="N48" s="36"/>
       <c r="O48" s="33"/>
       <c r="P48" s="46"/>
       <c r="Q48" s="16" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B49" s="30" t="str">
         <f>_xll.qlMakeDatedOIS(,E49,F49,OvernightIndex,0,,,,EvaluationDate)</f>
-        <v>obj_00278#0000</v>
+        <v>obj_00488#0000</v>
       </c>
       <c r="C49" s="10" t="b">
         <f>_xll.qlInstrumentSetPricingEngine(B49,OisEngine)</f>
@@ -11205,33 +11203,33 @@
         <v>23</v>
       </c>
       <c r="E49" s="55">
-        <f t="shared" si="12"/>
-        <v>41754</v>
+        <f t="shared" si="13"/>
+        <v>41766</v>
       </c>
       <c r="F49" s="24">
         <f>_xll.qlCalendarAdvance(Calendar,SettlementDate,D49,"mf",TRUE)</f>
-        <v>42121</v>
+        <v>42131</v>
       </c>
       <c r="G49" s="36"/>
       <c r="H49" s="33"/>
       <c r="I49" s="46"/>
       <c r="J49" s="32">
-        <f t="shared" si="20"/>
-        <v>5.483E-3</v>
+        <f t="shared" si="21"/>
+        <v>5.4774911031293646E-3</v>
       </c>
       <c r="K49" s="134">
-        <f t="shared" si="17"/>
-        <v>367</v>
+        <f t="shared" si="18"/>
+        <v>365</v>
       </c>
       <c r="L49" s="3">
         <f>_xll.qlOvernightIndexedSwapFairRate(B49,_xll.ohTrigger(C49,InterestRatesTrigger))</f>
-        <v>1.2399999999967541E-3</v>
+        <v>1.2899999999996363E-3</v>
       </c>
       <c r="N49" s="73"/>
       <c r="O49" s="74"/>
       <c r="P49" s="75"/>
       <c r="Q49" s="14" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#NUM!</v>
       </c>
     </row>
@@ -11265,7 +11263,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -11320,22 +11318,22 @@
       <c r="H2" s="168"/>
       <c r="I2" s="171"/>
       <c r="J2" s="172" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K2" s="170"/>
       <c r="L2" s="191" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M2" s="170"/>
       <c r="N2" s="171" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="172" t="s">
         <v>77</v>
       </c>
-      <c r="O2" s="172" t="s">
-        <v>78</v>
-      </c>
-      <c r="P2" s="239">
+      <c r="P2" s="233">
         <f>_xll.ohTrigger(O3:O7)</f>
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -11343,7 +11341,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="208" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="203" t="str">
         <f t="shared" ref="C3:C7" si="0">Currency&amp;$B3&amp;"_SYNTH"&amp;Tenor1M&amp;QuoteSuffix</f>
@@ -11351,7 +11349,7 @@
       </c>
       <c r="D3" s="204" t="str">
         <f>_xll.qlSimpleQuote(C3,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USDSND_SYNTH1M_Quote#0000</v>
+        <v>USDSND_SYNTH1M_Quote#0001</v>
       </c>
       <c r="E3" s="205" t="str">
         <f>_xll.ohRangeRetrieveError(D3)</f>
@@ -11360,11 +11358,11 @@
       <c r="F3" s="202"/>
       <c r="H3" s="206"/>
       <c r="I3" s="176" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J3" s="177">
         <f>Calculation!$G34</f>
-        <v>1.4640914902387782E-3</v>
+        <v>1.5222117163012955E-3</v>
       </c>
       <c r="K3" s="169"/>
       <c r="L3" s="182">
@@ -11373,11 +11371,11 @@
       <c r="M3" s="153"/>
       <c r="N3" s="185">
         <f t="array" ref="N3:N24">QuoteLive</f>
-        <v>1.4640914902387782E-3</v>
+        <v>1.5222117163012955E-3</v>
       </c>
       <c r="O3" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D3,ROUND(N3,6),EvaluationDate)</f>
-        <v>1.464E-3</v>
+        <v>0</v>
       </c>
       <c r="P3" s="207"/>
     </row>
@@ -11387,7 +11385,7 @@
         <v>1M</v>
       </c>
       <c r="B4" s="208" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="203" t="str">
         <f t="shared" si="0"/>
@@ -11395,7 +11393,7 @@
       </c>
       <c r="D4" s="204" t="str">
         <f>_xll.qlSimpleQuote(C4,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USDSWD_SYNTH1M_Quote#0000</v>
+        <v>USDSWD_SYNTH1M_Quote#0001</v>
       </c>
       <c r="E4" s="205" t="str">
         <f>_xll.ohRangeRetrieveError(D4)</f>
@@ -11404,11 +11402,11 @@
       <c r="F4" s="202"/>
       <c r="H4" s="206"/>
       <c r="I4" s="176" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J4" s="177">
         <f>Calculation!$G35</f>
-        <v>1.4638049627451184E-3</v>
+        <v>1.5189845194861083E-3</v>
       </c>
       <c r="K4" s="169"/>
       <c r="L4" s="182">
@@ -11416,18 +11414,18 @@
       </c>
       <c r="M4" s="153"/>
       <c r="N4" s="185">
-        <v>1.4638049627451184E-3</v>
+        <v>1.5189845194861083E-3</v>
       </c>
       <c r="O4" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D4,ROUND(N4,6),EvaluationDate)</f>
-        <v>1.464E-3</v>
+        <v>0</v>
       </c>
       <c r="P4" s="207"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="219"/>
       <c r="B5" s="208" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="203" t="str">
         <f t="shared" si="0"/>
@@ -11435,7 +11433,7 @@
       </c>
       <c r="D5" s="204" t="str">
         <f>_xll.qlSimpleQuote(C5,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD2WD_SYNTH1M_Quote#0000</v>
+        <v>USD2WD_SYNTH1M_Quote#0001</v>
       </c>
       <c r="E5" s="205" t="str">
         <f>_xll.ohRangeRetrieveError(D5)</f>
@@ -11444,11 +11442,11 @@
       <c r="F5" s="202"/>
       <c r="H5" s="206"/>
       <c r="I5" s="176" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="177">
         <f>Calculation!$G36</f>
-        <v>1.5033035367629133E-3</v>
+        <v>1.515219457614193E-3</v>
       </c>
       <c r="K5" s="169"/>
       <c r="L5" s="182">
@@ -11456,18 +11454,18 @@
       </c>
       <c r="M5" s="153"/>
       <c r="N5" s="185">
-        <v>1.5033035367629133E-3</v>
+        <v>1.515219457614193E-3</v>
       </c>
       <c r="O5" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D5,ROUND(N5,6),EvaluationDate)</f>
-        <v>1.503E-3</v>
+        <v>0</v>
       </c>
       <c r="P5" s="207"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="219"/>
       <c r="B6" s="208" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="203" t="str">
         <f t="shared" si="0"/>
@@ -11475,7 +11473,7 @@
       </c>
       <c r="D6" s="204" t="str">
         <f>_xll.qlSimpleQuote(C6,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD3WD_SYNTH1M_Quote#0000</v>
+        <v>USD3WD_SYNTH1M_Quote#0001</v>
       </c>
       <c r="E6" s="205" t="str">
         <f>_xll.ohRangeRetrieveError(D6)</f>
@@ -11484,11 +11482,11 @@
       <c r="F6" s="202"/>
       <c r="H6" s="206"/>
       <c r="I6" s="178" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J6" s="179">
         <f>Calculation!$G37</f>
-        <v>1.5128021123447842E-3</v>
+        <v>1.5114543904398529E-3</v>
       </c>
       <c r="K6" s="169"/>
       <c r="L6" s="183">
@@ -11496,18 +11494,18 @@
       </c>
       <c r="M6" s="153"/>
       <c r="N6" s="187">
-        <v>1.5128021123447842E-3</v>
+        <v>1.5114543904398529E-3</v>
       </c>
       <c r="O6" s="188">
         <f>_xll.qlSimpleQuoteSetValue(D6,ROUND(N6,6),EvaluationDate)</f>
-        <v>1.513E-3</v>
+        <v>0</v>
       </c>
       <c r="P6" s="207"/>
     </row>
     <row r="7" spans="1:16" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="219"/>
       <c r="B7" s="209" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="210" t="str">
         <f t="shared" si="0"/>
@@ -11515,7 +11513,7 @@
       </c>
       <c r="D7" s="210" t="str">
         <f>_xll.qlSimpleQuote(C7,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD1MD_SYNTH1M_Quote#0000</v>
+        <v>USD1MD_SYNTH1M_Quote#0001</v>
       </c>
       <c r="E7" s="211" t="str">
         <f>_xll.ohRangeRetrieveError(D7)</f>
@@ -11524,11 +11522,11 @@
       <c r="F7" s="202"/>
       <c r="H7" s="206"/>
       <c r="I7" s="180" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J7" s="181">
         <f>Calculation!$G38</f>
-        <v>1.5229999999999998E-3</v>
+        <v>1.505E-3</v>
       </c>
       <c r="K7" s="169"/>
       <c r="L7" s="184">
@@ -11536,11 +11534,11 @@
       </c>
       <c r="M7" s="153"/>
       <c r="N7" s="189">
-        <v>1.5229999999999998E-3</v>
+        <v>1.505E-3</v>
       </c>
       <c r="O7" s="190">
         <f>_xll.qlSimpleQuoteSetValue(D7,ROUND(N7,6),EvaluationDate)</f>
-        <v>1.523E-3</v>
+        <v>0</v>
       </c>
       <c r="P7" s="207"/>
     </row>
@@ -11549,7 +11547,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="212" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="203" t="str">
         <f t="shared" ref="C8:C14" si="1">Currency&amp;$B8&amp;"_SYNTH"&amp;Tenor3M&amp;QuoteSuffix</f>
@@ -11557,7 +11555,7 @@
       </c>
       <c r="D8" s="213" t="str">
         <f>_xll.qlSimpleQuote(C8,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USDSND_SYNTH3M_Quote#0000</v>
+        <v>USDSND_SYNTH3M_Quote#0001</v>
       </c>
       <c r="E8" s="214" t="str">
         <f>_xll.ohRangeRetrieveError(D8)</f>
@@ -11566,11 +11564,11 @@
       <c r="F8" s="215"/>
       <c r="H8" s="206"/>
       <c r="I8" s="176" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="177">
         <f>Calculation!$H34</f>
-        <v>2.3206693711853759E-3</v>
+        <v>2.3587517391352054E-3</v>
       </c>
       <c r="K8" s="169"/>
       <c r="L8" s="182">
@@ -11578,15 +11576,15 @@
       </c>
       <c r="M8" s="153"/>
       <c r="N8" s="185">
-        <v>2.3206693711853759E-3</v>
+        <v>2.3587517391352054E-3</v>
       </c>
       <c r="O8" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D8,ROUND(N8,6),EvaluationDate)</f>
-        <v>2.3210000000000001E-3</v>
-      </c>
-      <c r="P8" s="240">
+        <v>0</v>
+      </c>
+      <c r="P8" s="234">
         <f>_xll.ohTrigger(O8:O14)</f>
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -11595,7 +11593,7 @@
         <v>3M</v>
       </c>
       <c r="B9" s="208" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="203" t="str">
         <f t="shared" si="1"/>
@@ -11603,7 +11601,7 @@
       </c>
       <c r="D9" s="203" t="str">
         <f>_xll.qlSimpleQuote(C9,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USDSWD_SYNTH3M_Quote#0000</v>
+        <v>USDSWD_SYNTH3M_Quote#0001</v>
       </c>
       <c r="E9" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D9)</f>
@@ -11612,11 +11610,11 @@
       <c r="F9" s="215"/>
       <c r="H9" s="206"/>
       <c r="I9" s="176" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J9" s="177">
         <f>Calculation!$H35</f>
-        <v>2.3132632711997509E-3</v>
+        <v>2.3428157445206771E-3</v>
       </c>
       <c r="K9" s="169"/>
       <c r="L9" s="182">
@@ -11624,18 +11622,18 @@
       </c>
       <c r="M9" s="153"/>
       <c r="N9" s="185">
-        <v>2.3132632711997509E-3</v>
+        <v>2.3428157445206771E-3</v>
       </c>
       <c r="O9" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D9,ROUND(N9,6),EvaluationDate)</f>
-        <v>2.313E-3</v>
+        <v>0</v>
       </c>
       <c r="P9" s="207"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="221"/>
       <c r="B10" s="217" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="203" t="str">
         <f t="shared" si="1"/>
@@ -11643,7 +11641,7 @@
       </c>
       <c r="D10" s="203" t="str">
         <f>_xll.qlSimpleQuote(C10,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD2WD_SYNTH3M_Quote#0000</v>
+        <v>USD2WD_SYNTH3M_Quote#0001</v>
       </c>
       <c r="E10" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D10)</f>
@@ -11652,11 +11650,11 @@
       <c r="F10" s="215"/>
       <c r="H10" s="206"/>
       <c r="I10" s="176" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" s="177">
         <f>Calculation!$H36</f>
-        <v>2.3409251436399916E-3</v>
+        <v>2.3251819187032133E-3</v>
       </c>
       <c r="K10" s="169"/>
       <c r="L10" s="182">
@@ -11664,18 +11662,18 @@
       </c>
       <c r="M10" s="153"/>
       <c r="N10" s="185">
-        <v>2.3409251436399916E-3</v>
+        <v>2.3251819187032133E-3</v>
       </c>
       <c r="O10" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D10,ROUND(N10,6),EvaluationDate)</f>
-        <v>2.3410000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="P10" s="207"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="222"/>
       <c r="B11" s="217" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="203" t="str">
         <f t="shared" si="1"/>
@@ -11683,7 +11681,7 @@
       </c>
       <c r="D11" s="203" t="str">
         <f>_xll.qlSimpleQuote(C11,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD3WD_SYNTH3M_Quote#0000</v>
+        <v>USD3WD_SYNTH3M_Quote#0001</v>
       </c>
       <c r="E11" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D11)</f>
@@ -11692,11 +11690,11 @@
       <c r="F11" s="215"/>
       <c r="H11" s="206"/>
       <c r="I11" s="176" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J11" s="177">
         <f>Calculation!$H37</f>
-        <v>2.339379354368616E-3</v>
+        <v>2.3085799595437008E-3</v>
       </c>
       <c r="K11" s="169"/>
       <c r="L11" s="182">
@@ -11704,18 +11702,18 @@
       </c>
       <c r="M11" s="153"/>
       <c r="N11" s="185">
-        <v>2.339379354368616E-3</v>
+        <v>2.3085799595437008E-3</v>
       </c>
       <c r="O11" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D11,ROUND(N11,6),EvaluationDate)</f>
-        <v>2.3389999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="P11" s="207"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="222"/>
       <c r="B12" s="217" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="203" t="str">
         <f t="shared" si="1"/>
@@ -11723,7 +11721,7 @@
       </c>
       <c r="D12" s="203" t="str">
         <f>_xll.qlSimpleQuote(C12,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD1MD_SYNTH3M_Quote#0000</v>
+        <v>USD1MD_SYNTH3M_Quote#0001</v>
       </c>
       <c r="E12" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D12)</f>
@@ -11732,11 +11730,11 @@
       <c r="F12" s="215"/>
       <c r="H12" s="206"/>
       <c r="I12" s="176" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J12" s="177">
         <f>Calculation!$H38</f>
-        <v>2.3338226551260048E-3</v>
+        <v>2.2825201502615707E-3</v>
       </c>
       <c r="K12" s="169"/>
       <c r="L12" s="182">
@@ -11744,18 +11742,18 @@
       </c>
       <c r="M12" s="153"/>
       <c r="N12" s="185">
-        <v>2.3338226551260048E-3</v>
+        <v>2.2825201502615707E-3</v>
       </c>
       <c r="O12" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D12,ROUND(N12,6),EvaluationDate)</f>
-        <v>2.3340000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="P12" s="207"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="222"/>
       <c r="B13" s="217" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="203" t="str">
         <f t="shared" si="1"/>
@@ -11763,7 +11761,7 @@
       </c>
       <c r="D13" s="203" t="str">
         <f>_xll.qlSimpleQuote(C13,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD2MD_SYNTH3M_Quote#0000</v>
+        <v>USD2MD_SYNTH3M_Quote#0001</v>
       </c>
       <c r="E13" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D13)</f>
@@ -11772,11 +11770,11 @@
       <c r="F13" s="215"/>
       <c r="H13" s="206"/>
       <c r="I13" s="176" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J13" s="177">
         <f>Calculation!$H39</f>
-        <v>2.3086033575903308E-3</v>
+        <v>2.2535067435047801E-3</v>
       </c>
       <c r="K13" s="169"/>
       <c r="L13" s="182">
@@ -11784,18 +11782,18 @@
       </c>
       <c r="M13" s="153"/>
       <c r="N13" s="185">
-        <v>2.3086033575903308E-3</v>
+        <v>2.2535067435047801E-3</v>
       </c>
       <c r="O13" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D13,ROUND(N13,6),EvaluationDate)</f>
-        <v>2.3089999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="P13" s="207"/>
     </row>
     <row r="14" spans="1:16" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="224"/>
       <c r="B14" s="209" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="210" t="str">
         <f t="shared" si="1"/>
@@ -11803,7 +11801,7 @@
       </c>
       <c r="D14" s="210" t="str">
         <f>_xll.qlSimpleQuote(C14,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD3MD_SYNTH3M_Quote#0000</v>
+        <v>USD3MD_SYNTH3M_Quote#0001</v>
       </c>
       <c r="E14" s="225" t="str">
         <f>_xll.ohRangeRetrieveError(D14)</f>
@@ -11812,11 +11810,11 @@
       <c r="F14" s="215"/>
       <c r="H14" s="223"/>
       <c r="I14" s="180" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J14" s="181">
         <f>Calculation!$H40</f>
-        <v>2.2875000000000009E-3</v>
+        <v>2.2285000000000022E-3</v>
       </c>
       <c r="K14" s="223"/>
       <c r="L14" s="184">
@@ -11824,11 +11822,11 @@
       </c>
       <c r="M14" s="223"/>
       <c r="N14" s="189">
-        <v>2.2875000000000009E-3</v>
+        <v>2.2285000000000022E-3</v>
       </c>
       <c r="O14" s="190">
         <f>_xll.qlSimpleQuoteSetValue(D14,ROUND(N14,6),EvaluationDate)</f>
-        <v>2.2880000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="P14" s="223"/>
     </row>
@@ -11837,7 +11835,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="212" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="203" t="str">
         <f t="shared" ref="C15:C24" si="2">Currency&amp;$B15&amp;"_SYNTH"&amp;Tenor6M&amp;QuoteSuffix</f>
@@ -11845,7 +11843,7 @@
       </c>
       <c r="D15" s="213" t="str">
         <f>_xll.qlSimpleQuote(C15,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USDSND_SYNTH6M_Quote#0000</v>
+        <v>USDSND_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E15" s="214" t="str">
         <f>_xll.ohRangeRetrieveError(D15)</f>
@@ -11854,11 +11852,11 @@
       <c r="F15" s="215"/>
       <c r="H15" s="206"/>
       <c r="I15" s="176" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J15" s="177">
         <f>Calculation!$I34</f>
-        <v>3.340640475011732E-3</v>
+        <v>3.4120803864403854E-3</v>
       </c>
       <c r="K15" s="169"/>
       <c r="L15" s="182">
@@ -11866,15 +11864,15 @@
       </c>
       <c r="M15" s="153"/>
       <c r="N15" s="185">
-        <v>3.340640475011732E-3</v>
+        <v>3.4120803864403854E-3</v>
       </c>
       <c r="O15" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D15,ROUND(N15,6),EvaluationDate)</f>
-        <v>3.3409999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="P15" s="207">
         <f>_xll.ohTrigger(O15:O24)</f>
-        <v>1</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -11883,7 +11881,7 @@
         <v>6M</v>
       </c>
       <c r="B16" s="208" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="203" t="str">
         <f t="shared" si="2"/>
@@ -11891,7 +11889,7 @@
       </c>
       <c r="D16" s="203" t="str">
         <f>_xll.qlSimpleQuote(C16,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USDSWD_SYNTH6M_Quote#0000</v>
+        <v>USDSWD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E16" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D16)</f>
@@ -11900,11 +11898,11 @@
       <c r="F16" s="215"/>
       <c r="H16" s="206"/>
       <c r="I16" s="176" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J16" s="177">
         <f>Calculation!$I35</f>
-        <v>3.330246221872263E-3</v>
+        <v>3.3959398777909954E-3</v>
       </c>
       <c r="K16" s="169"/>
       <c r="L16" s="182">
@@ -11912,18 +11910,18 @@
       </c>
       <c r="M16" s="153"/>
       <c r="N16" s="185">
-        <v>3.330246221872263E-3</v>
+        <v>3.3959398777909954E-3</v>
       </c>
       <c r="O16" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D16,ROUND(N16,6),EvaluationDate)</f>
-        <v>3.3300000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="P16" s="207"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="221"/>
       <c r="B17" s="217" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="203" t="str">
         <f t="shared" si="2"/>
@@ -11931,7 +11929,7 @@
       </c>
       <c r="D17" s="203" t="str">
         <f>_xll.qlSimpleQuote(C17,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD2WD_SYNTH6M_Quote#0000</v>
+        <v>USD2WD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E17" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D17)</f>
@@ -11940,11 +11938,11 @@
       <c r="F17" s="215"/>
       <c r="H17" s="206"/>
       <c r="I17" s="176" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J17" s="177">
         <f>Calculation!$I36</f>
-        <v>3.352579888468181E-3</v>
+        <v>3.377660840774524E-3</v>
       </c>
       <c r="K17" s="169"/>
       <c r="L17" s="182">
@@ -11952,18 +11950,18 @@
       </c>
       <c r="M17" s="153"/>
       <c r="N17" s="185">
-        <v>3.352579888468181E-3</v>
+        <v>3.377660840774524E-3</v>
       </c>
       <c r="O17" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D17,ROUND(N17,6),EvaluationDate)</f>
-        <v>3.3530000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="P17" s="207"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="222"/>
       <c r="B18" s="217" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="203" t="str">
         <f t="shared" si="2"/>
@@ -11971,7 +11969,7 @@
       </c>
       <c r="D18" s="203" t="str">
         <f>_xll.qlSimpleQuote(C18,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD3WD_SYNTH6M_Quote#0000</v>
+        <v>USD3WD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E18" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D18)</f>
@@ -11980,11 +11978,11 @@
       <c r="F18" s="215"/>
       <c r="H18" s="206"/>
       <c r="I18" s="176" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J18" s="177">
         <f>Calculation!$I37</f>
-        <v>3.3455799724841791E-3</v>
+        <v>3.3599757811172844E-3</v>
       </c>
       <c r="K18" s="169"/>
       <c r="L18" s="182">
@@ -11992,18 +11990,18 @@
       </c>
       <c r="M18" s="153"/>
       <c r="N18" s="185">
-        <v>3.3455799724841791E-3</v>
+        <v>3.3599757811172844E-3</v>
       </c>
       <c r="O18" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D18,ROUND(N18,6),EvaluationDate)</f>
-        <v>3.346E-3</v>
+        <v>0</v>
       </c>
       <c r="P18" s="207"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="222"/>
       <c r="B19" s="217" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="203" t="str">
         <f t="shared" si="2"/>
@@ -12011,7 +12009,7 @@
       </c>
       <c r="D19" s="203" t="str">
         <f>_xll.qlSimpleQuote(C19,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD1MD_SYNTH6M_Quote#0000</v>
+        <v>USD1MD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E19" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D19)</f>
@@ -12020,11 +12018,11 @@
       <c r="F19" s="215"/>
       <c r="H19" s="206"/>
       <c r="I19" s="176" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" s="177">
         <f>Calculation!$I38</f>
-        <v>3.3311980911429088E-3</v>
+        <v>3.3310404652665171E-3</v>
       </c>
       <c r="K19" s="169"/>
       <c r="L19" s="182">
@@ -12032,18 +12030,18 @@
       </c>
       <c r="M19" s="153"/>
       <c r="N19" s="185">
-        <v>3.3311980911429088E-3</v>
+        <v>3.3310404652665171E-3</v>
       </c>
       <c r="O19" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D19,ROUND(N19,6),EvaluationDate)</f>
-        <v>3.3310000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="P19" s="207"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="222"/>
       <c r="B20" s="217" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="203" t="str">
         <f t="shared" si="2"/>
@@ -12051,7 +12049,7 @@
       </c>
       <c r="D20" s="203" t="str">
         <f>_xll.qlSimpleQuote(C20,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD2MD_SYNTH6M_Quote#0000</v>
+        <v>USD2MD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E20" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D20)</f>
@@ -12060,11 +12058,11 @@
       <c r="F20" s="215"/>
       <c r="H20" s="206"/>
       <c r="I20" s="176" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J20" s="177">
         <f>Calculation!$I39</f>
-        <v>3.2812219125275088E-3</v>
+        <v>3.2903130940546733E-3</v>
       </c>
       <c r="K20" s="169"/>
       <c r="L20" s="182">
@@ -12072,18 +12070,18 @@
       </c>
       <c r="M20" s="153"/>
       <c r="N20" s="185">
-        <v>3.2812219125275088E-3</v>
+        <v>3.2903130940546733E-3</v>
       </c>
       <c r="O20" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D20,ROUND(N20,6),EvaluationDate)</f>
-        <v>3.2810000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="P20" s="207"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="222"/>
       <c r="B21" s="217" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="203" t="str">
         <f t="shared" si="2"/>
@@ -12091,7 +12089,7 @@
       </c>
       <c r="D21" s="203" t="str">
         <f>_xll.qlSimpleQuote(C21,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD3MD_SYNTH6M_Quote#0000</v>
+        <v>USD3MD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E21" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D21)</f>
@@ -12100,11 +12098,11 @@
       <c r="F21" s="215"/>
       <c r="H21" s="206"/>
       <c r="I21" s="176" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J21" s="177">
         <f>Calculation!$I40</f>
-        <v>3.2322337032325956E-3</v>
+        <v>3.2441648743179274E-3</v>
       </c>
       <c r="K21" s="169"/>
       <c r="L21" s="182">
@@ -12112,18 +12110,18 @@
       </c>
       <c r="M21" s="153"/>
       <c r="N21" s="185">
-        <v>3.2322337032325956E-3</v>
+        <v>3.2441648743179274E-3</v>
       </c>
       <c r="O21" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D21,ROUND(N21,6),EvaluationDate)</f>
-        <v>3.2320000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="P21" s="207"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="222"/>
       <c r="B22" s="217" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="203" t="str">
         <f t="shared" si="2"/>
@@ -12131,7 +12129,7 @@
       </c>
       <c r="D22" s="203" t="str">
         <f>_xll.qlSimpleQuote(C22,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD4MD_SYNTH6M_Quote#0000</v>
+        <v>USD4MD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E22" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D22)</f>
@@ -12140,11 +12138,11 @@
       <c r="F22" s="215"/>
       <c r="H22" s="206"/>
       <c r="I22" s="176" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J22" s="177">
         <f>Calculation!$I41</f>
-        <v>3.2141301064413756E-3</v>
+        <v>3.2184244950372947E-3</v>
       </c>
       <c r="K22" s="169"/>
       <c r="L22" s="182">
@@ -12152,18 +12150,18 @@
       </c>
       <c r="M22" s="153"/>
       <c r="N22" s="185">
-        <v>3.2141301064413756E-3</v>
+        <v>3.2184244950372947E-3</v>
       </c>
       <c r="O22" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D22,ROUND(N22,6),EvaluationDate)</f>
-        <v>3.2139999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="P22" s="207"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="222"/>
       <c r="B23" s="217" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="203" t="str">
         <f t="shared" si="2"/>
@@ -12171,7 +12169,7 @@
       </c>
       <c r="D23" s="203" t="str">
         <f>_xll.qlSimpleQuote(C23,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD5MD_SYNTH6M_Quote#0000</v>
+        <v>USD5MD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E23" s="216" t="str">
         <f>_xll.ohRangeRetrieveError(D23)</f>
@@ -12180,11 +12178,11 @@
       <c r="F23" s="215"/>
       <c r="H23" s="206"/>
       <c r="I23" s="176" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J23" s="177">
         <f>Calculation!$I42</f>
-        <v>3.2097795269059441E-3</v>
+        <v>3.2076942677200346E-3</v>
       </c>
       <c r="K23" s="169"/>
       <c r="L23" s="182">
@@ -12192,18 +12190,18 @@
       </c>
       <c r="M23" s="153"/>
       <c r="N23" s="185">
-        <v>3.2097795269059441E-3</v>
+        <v>3.2076942677200346E-3</v>
       </c>
       <c r="O23" s="186">
         <f>_xll.qlSimpleQuoteSetValue(D23,ROUND(N23,6),EvaluationDate)</f>
-        <v>3.2100000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="P23" s="207"/>
     </row>
     <row r="24" spans="1:16" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="224"/>
       <c r="B24" s="209" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="210" t="str">
         <f t="shared" si="2"/>
@@ -12211,7 +12209,7 @@
       </c>
       <c r="D24" s="210" t="str">
         <f>_xll.qlSimpleQuote(C24,,RateTickValue,Permanent,EvaluationDate,ObjectOverwrite)</f>
-        <v>USD6MD_SYNTH6M_Quote#0000</v>
+        <v>USD6MD_SYNTH6M_Quote#0001</v>
       </c>
       <c r="E24" s="225" t="str">
         <f>_xll.ohRangeRetrieveError(D24)</f>
@@ -12220,11 +12218,11 @@
       <c r="F24" s="226"/>
       <c r="H24" s="227"/>
       <c r="I24" s="180" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J24" s="181">
         <f>Calculation!$I43</f>
-        <v>3.2280000000000043E-3</v>
+        <v>3.2161182643953038E-3</v>
       </c>
       <c r="K24" s="228"/>
       <c r="L24" s="184">
@@ -12232,11 +12230,11 @@
       </c>
       <c r="M24" s="229"/>
       <c r="N24" s="189">
-        <v>3.2280000000000043E-3</v>
+        <v>3.2161182643953038E-3</v>
       </c>
       <c r="O24" s="190">
         <f>_xll.qlSimpleQuoteSetValue(D24,ROUND(N24,6),EvaluationDate)</f>
-        <v>3.228E-3</v>
+        <v>0</v>
       </c>
       <c r="P24" s="230"/>
     </row>

</xml_diff>